<commit_message>
added category model, changed lexical category to a field of category model, added has_grammar field to instrument map #72
</commit_message>
<xml_diff>
--- a/raw_data/Norwegian_WG/[Norwegian_WG].xlsx
+++ b/raw_data/Norwegian_WG/[Norwegian_WG].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="13040" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -6140,8 +6140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A411" workbookViewId="0">
-      <selection activeCell="I427" sqref="I427"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
fixed a bunch of dumb glosses
</commit_message>
<xml_diff>
--- a/raw_data/Norwegian_WG/[Norwegian_WG].xlsx
+++ b/raw_data/Norwegian_WG/[Norwegian_WG].xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3761" uniqueCount="1882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3761" uniqueCount="1886">
   <si>
     <t>item</t>
   </si>
@@ -4632,9 +4632,6 @@
     <t>sheep</t>
   </si>
   <si>
-    <t>brr (car audio)</t>
-  </si>
-  <si>
     <t>grrr</t>
   </si>
   <si>
@@ -5262,9 +5259,6 @@
     <t>bye bye</t>
   </si>
   <si>
-    <t>hey there</t>
-  </si>
-  <si>
     <t>hush</t>
   </si>
   <si>
@@ -5665,6 +5659,24 @@
   </si>
   <si>
     <t>same</t>
+  </si>
+  <si>
+    <t>quack quack</t>
+  </si>
+  <si>
+    <t>vroom</t>
+  </si>
+  <si>
+    <t>woof woof</t>
+  </si>
+  <si>
+    <t>yum yum</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>baa baa</t>
   </si>
 </sst>
 </file>
@@ -5737,8 +5749,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5786,7 +5818,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5798,6 +5830,16 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5809,6 +5851,16 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6140,8 +6192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L490"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6933,7 +6985,7 @@
         <v>1024</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>1024</v>
+        <v>1885</v>
       </c>
       <c r="J34" t="s">
         <v>528</v>
@@ -6959,7 +7011,7 @@
         <v>1025</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>1537</v>
+        <v>1881</v>
       </c>
       <c r="J35" t="s">
         <v>528</v>
@@ -6985,7 +7037,7 @@
         <v>1026</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>1026</v>
+        <v>1880</v>
       </c>
       <c r="J36" t="s">
         <v>528</v>
@@ -7011,7 +7063,7 @@
         <v>1027</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="J37" t="s">
         <v>528</v>
@@ -7063,7 +7115,7 @@
         <v>1029</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="J39" t="s">
         <v>528</v>
@@ -7089,7 +7141,7 @@
         <v>1030</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="J40" t="s">
         <v>528</v>
@@ -7115,7 +7167,7 @@
         <v>1031</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>1031</v>
+        <v>1883</v>
       </c>
       <c r="J41" t="s">
         <v>528</v>
@@ -7141,7 +7193,7 @@
         <v>1032</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="J42" t="s">
         <v>528</v>
@@ -7167,7 +7219,7 @@
         <v>1033</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>1033</v>
+        <v>1882</v>
       </c>
       <c r="J43" t="s">
         <v>528</v>
@@ -7193,7 +7245,7 @@
         <v>1034</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="J44" t="s">
         <v>529</v>
@@ -7219,7 +7271,7 @@
         <v>1035</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="J45" t="s">
         <v>529</v>
@@ -7245,7 +7297,7 @@
         <v>1036</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="J46" t="s">
         <v>529</v>
@@ -7271,7 +7323,7 @@
         <v>1037</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="J47" t="s">
         <v>529</v>
@@ -7323,7 +7375,7 @@
         <v>1039</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="J49" t="s">
         <v>529</v>
@@ -7349,7 +7401,7 @@
         <v>1040</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="J50" t="s">
         <v>529</v>
@@ -7375,7 +7427,7 @@
         <v>1041</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="J51" t="s">
         <v>529</v>
@@ -7401,7 +7453,7 @@
         <v>1042</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="J52" t="s">
         <v>529</v>
@@ -7453,7 +7505,7 @@
         <v>1044</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="J54" t="s">
         <v>529</v>
@@ -7479,7 +7531,7 @@
         <v>1045</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="J55" t="s">
         <v>529</v>
@@ -7505,7 +7557,7 @@
         <v>1046</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="J56" t="s">
         <v>529</v>
@@ -7531,7 +7583,7 @@
         <v>1047</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="J57" t="s">
         <v>529</v>
@@ -7557,7 +7609,7 @@
         <v>1048</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="J58" t="s">
         <v>529</v>
@@ -7583,7 +7635,7 @@
         <v>1049</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="J59" t="s">
         <v>529</v>
@@ -7609,7 +7661,7 @@
         <v>1050</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="J60" t="s">
         <v>529</v>
@@ -7635,7 +7687,7 @@
         <v>1051</v>
       </c>
       <c r="I61" s="11" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="J61" t="s">
         <v>529</v>
@@ -7661,7 +7713,7 @@
         <v>1052</v>
       </c>
       <c r="I62" s="11" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="J62" t="s">
         <v>529</v>
@@ -7687,7 +7739,7 @@
         <v>1053</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="J63" t="s">
         <v>529</v>
@@ -7713,7 +7765,7 @@
         <v>1054</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="J64" t="s">
         <v>529</v>
@@ -7739,7 +7791,7 @@
         <v>1055</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="J65" t="s">
         <v>529</v>
@@ -7765,7 +7817,7 @@
         <v>1056</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="J66" t="s">
         <v>529</v>
@@ -7791,7 +7843,7 @@
         <v>1057</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="J67" t="s">
         <v>529</v>
@@ -7817,7 +7869,7 @@
         <v>1058</v>
       </c>
       <c r="I68" s="11" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="J68" t="s">
         <v>529</v>
@@ -7843,7 +7895,7 @@
         <v>1059</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="J69" t="s">
         <v>529</v>
@@ -7869,7 +7921,7 @@
         <v>1060</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="J70" t="s">
         <v>529</v>
@@ -7895,7 +7947,7 @@
         <v>1061</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="J71" t="s">
         <v>529</v>
@@ -7947,7 +7999,7 @@
         <v>1063</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="J73" t="s">
         <v>529</v>
@@ -7973,7 +8025,7 @@
         <v>1064</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="J74" t="s">
         <v>529</v>
@@ -7999,7 +8051,7 @@
         <v>1065</v>
       </c>
       <c r="I75" s="11" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="J75" t="s">
         <v>529</v>
@@ -8051,7 +8103,7 @@
         <v>1067</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="J77" t="s">
         <v>529</v>
@@ -8077,7 +8129,7 @@
         <v>1068</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="J78" t="s">
         <v>529</v>
@@ -8103,7 +8155,7 @@
         <v>1069</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="J79" t="s">
         <v>529</v>
@@ -8129,7 +8181,7 @@
         <v>1070</v>
       </c>
       <c r="I80" s="11" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="J80" t="s">
         <v>529</v>
@@ -8155,7 +8207,7 @@
         <v>1071</v>
       </c>
       <c r="I81" s="11" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="J81" t="s">
         <v>529</v>
@@ -8181,7 +8233,7 @@
         <v>1072</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="J82" t="s">
         <v>529</v>
@@ -8207,7 +8259,7 @@
         <v>1073</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="J83" t="s">
         <v>529</v>
@@ -8233,7 +8285,7 @@
         <v>1074</v>
       </c>
       <c r="I84" s="11" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="J84" t="s">
         <v>529</v>
@@ -8259,7 +8311,7 @@
         <v>1075</v>
       </c>
       <c r="I85" s="11" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="J85" t="s">
         <v>529</v>
@@ -8285,7 +8337,7 @@
         <v>1076</v>
       </c>
       <c r="I86" s="11" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="J86" t="s">
         <v>529</v>
@@ -8311,7 +8363,7 @@
         <v>1077</v>
       </c>
       <c r="I87" s="11" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="J87" t="s">
         <v>529</v>
@@ -8337,7 +8389,7 @@
         <v>1078</v>
       </c>
       <c r="I88" s="11" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="J88" t="s">
         <v>529</v>
@@ -8363,7 +8415,7 @@
         <v>1079</v>
       </c>
       <c r="I89" s="11" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="J89" t="s">
         <v>529</v>
@@ -8389,7 +8441,7 @@
         <v>1080</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="J90" t="s">
         <v>529</v>
@@ -8415,7 +8467,7 @@
         <v>1081</v>
       </c>
       <c r="I91" s="11" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="J91" t="s">
         <v>529</v>
@@ -8441,7 +8493,7 @@
         <v>1082</v>
       </c>
       <c r="I92" s="11" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="J92" t="s">
         <v>529</v>
@@ -8467,7 +8519,7 @@
         <v>1083</v>
       </c>
       <c r="I93" s="11" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
       <c r="J93" t="s">
         <v>529</v>
@@ -8493,7 +8545,7 @@
         <v>1084</v>
       </c>
       <c r="I94" s="11" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="J94" t="s">
         <v>529</v>
@@ -8519,7 +8571,7 @@
         <v>1085</v>
       </c>
       <c r="I95" s="11" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="J95" t="s">
         <v>529</v>
@@ -8545,7 +8597,7 @@
         <v>1086</v>
       </c>
       <c r="I96" s="11" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="J96" t="s">
         <v>529</v>
@@ -8571,7 +8623,7 @@
         <v>1087</v>
       </c>
       <c r="I97" s="11" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="J97" t="s">
         <v>529</v>
@@ -8597,7 +8649,7 @@
         <v>1088</v>
       </c>
       <c r="I98" s="11" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="J98" t="s">
         <v>529</v>
@@ -8623,7 +8675,7 @@
         <v>1089</v>
       </c>
       <c r="I99" s="11" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
       <c r="J99" t="s">
         <v>529</v>
@@ -8649,7 +8701,7 @@
         <v>1090</v>
       </c>
       <c r="I100" s="11" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
       <c r="J100" t="s">
         <v>529</v>
@@ -8701,7 +8753,7 @@
         <v>1092</v>
       </c>
       <c r="I102" s="11" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="J102" t="s">
         <v>529</v>
@@ -8727,7 +8779,7 @@
         <v>1093</v>
       </c>
       <c r="I103" s="11" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="J103" t="s">
         <v>529</v>
@@ -8753,7 +8805,7 @@
         <v>1094</v>
       </c>
       <c r="I104" s="11" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
       <c r="J104" t="s">
         <v>529</v>
@@ -8779,7 +8831,7 @@
         <v>1042</v>
       </c>
       <c r="I105" s="11" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="J105" t="s">
         <v>529</v>
@@ -8805,7 +8857,7 @@
         <v>1095</v>
       </c>
       <c r="I106" s="11" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="J106" t="s">
         <v>529</v>
@@ -8831,7 +8883,7 @@
         <v>1096</v>
       </c>
       <c r="I107" s="11" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="J107" t="s">
         <v>529</v>
@@ -8857,7 +8909,7 @@
         <v>1097</v>
       </c>
       <c r="I108" s="11" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="J108" t="s">
         <v>529</v>
@@ -8909,7 +8961,7 @@
         <v>1099</v>
       </c>
       <c r="I110" s="11" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="J110" t="s">
         <v>529</v>
@@ -8935,7 +8987,7 @@
         <v>1100</v>
       </c>
       <c r="I111" s="11" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="J111" t="s">
         <v>529</v>
@@ -8961,7 +9013,7 @@
         <v>1101</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="J112" t="s">
         <v>529</v>
@@ -8987,7 +9039,7 @@
         <v>1102</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="J113" t="s">
         <v>529</v>
@@ -9013,7 +9065,7 @@
         <v>1054</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="J114" t="s">
         <v>529</v>
@@ -9039,7 +9091,7 @@
         <v>1103</v>
       </c>
       <c r="I115" s="11" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="J115" t="s">
         <v>529</v>
@@ -9065,7 +9117,7 @@
         <v>1104</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="J116" t="s">
         <v>529</v>
@@ -9091,7 +9143,7 @@
         <v>1105</v>
       </c>
       <c r="I117" s="11" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="J117" t="s">
         <v>529</v>
@@ -9169,7 +9221,7 @@
         <v>1108</v>
       </c>
       <c r="I120" s="11" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="J120" t="s">
         <v>529</v>
@@ -9195,7 +9247,7 @@
         <v>1109</v>
       </c>
       <c r="I121" s="11" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="J121" t="s">
         <v>529</v>
@@ -9221,7 +9273,7 @@
         <v>1110</v>
       </c>
       <c r="I122" s="11" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="J122" t="s">
         <v>529</v>
@@ -9247,7 +9299,7 @@
         <v>1111</v>
       </c>
       <c r="I123" s="11" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="J123" t="s">
         <v>529</v>
@@ -9273,7 +9325,7 @@
         <v>1112</v>
       </c>
       <c r="I124" s="11" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="J124" t="s">
         <v>529</v>
@@ -9299,7 +9351,7 @@
         <v>1113</v>
       </c>
       <c r="I125" s="11" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="J125" t="s">
         <v>529</v>
@@ -9325,7 +9377,7 @@
         <v>1114</v>
       </c>
       <c r="I126" s="11" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="J126" t="s">
         <v>529</v>
@@ -9351,7 +9403,7 @@
         <v>1115</v>
       </c>
       <c r="I127" s="11" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="J127" t="s">
         <v>529</v>
@@ -9377,7 +9429,7 @@
         <v>1116</v>
       </c>
       <c r="I128" s="11" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="J128" t="s">
         <v>529</v>
@@ -9403,7 +9455,7 @@
         <v>1117</v>
       </c>
       <c r="I129" s="11" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="J129" t="s">
         <v>529</v>
@@ -9429,7 +9481,7 @@
         <v>1118</v>
       </c>
       <c r="I130" s="11" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="J130" t="s">
         <v>529</v>
@@ -9455,7 +9507,7 @@
         <v>1119</v>
       </c>
       <c r="I131" s="11" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="J131" t="s">
         <v>529</v>
@@ -9481,7 +9533,7 @@
         <v>1120</v>
       </c>
       <c r="I132" s="11" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="J132" t="s">
         <v>529</v>
@@ -9507,7 +9559,7 @@
         <v>1121</v>
       </c>
       <c r="I133" s="11" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="J133" t="s">
         <v>529</v>
@@ -9533,7 +9585,7 @@
         <v>1122</v>
       </c>
       <c r="I134" s="11" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="J134" t="s">
         <v>529</v>
@@ -9559,7 +9611,7 @@
         <v>1123</v>
       </c>
       <c r="I135" s="11" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="J135" t="s">
         <v>529</v>
@@ -9611,7 +9663,7 @@
         <v>1125</v>
       </c>
       <c r="I137" s="11" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="J137" t="s">
         <v>529</v>
@@ -9637,7 +9689,7 @@
         <v>1126</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="J138" t="s">
         <v>529</v>
@@ -9663,7 +9715,7 @@
         <v>1127</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="J139" t="s">
         <v>529</v>
@@ -9689,7 +9741,7 @@
         <v>1128</v>
       </c>
       <c r="I140" s="11" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="J140" t="s">
         <v>529</v>
@@ -9715,7 +9767,7 @@
         <v>1129</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="J141" t="s">
         <v>529</v>
@@ -9741,7 +9793,7 @@
         <v>1130</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="J142" t="s">
         <v>529</v>
@@ -9767,7 +9819,7 @@
         <v>1131</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="J143" t="s">
         <v>529</v>
@@ -9793,7 +9845,7 @@
         <v>1132</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="J144" t="s">
         <v>529</v>
@@ -9819,7 +9871,7 @@
         <v>1133</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="J145" t="s">
         <v>529</v>
@@ -9871,7 +9923,7 @@
         <v>1135</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="J147" t="s">
         <v>529</v>
@@ -9923,7 +9975,7 @@
         <v>1137</v>
       </c>
       <c r="I149" s="11" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="J149" t="s">
         <v>529</v>
@@ -9949,7 +10001,7 @@
         <v>1138</v>
       </c>
       <c r="I150" s="11" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="J150" t="s">
         <v>529</v>
@@ -9975,7 +10027,7 @@
         <v>1139</v>
       </c>
       <c r="I151" s="11" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="J151" t="s">
         <v>529</v>
@@ -10001,7 +10053,7 @@
         <v>1140</v>
       </c>
       <c r="I152" s="11" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="J152" t="s">
         <v>529</v>
@@ -10027,7 +10079,7 @@
         <v>1141</v>
       </c>
       <c r="I153" s="11" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="J153" t="s">
         <v>529</v>
@@ -10053,7 +10105,7 @@
         <v>1142</v>
       </c>
       <c r="I154" s="11" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="J154" t="s">
         <v>529</v>
@@ -10079,7 +10131,7 @@
         <v>1143</v>
       </c>
       <c r="I155" s="11" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="J155" t="s">
         <v>529</v>
@@ -10105,7 +10157,7 @@
         <v>1144</v>
       </c>
       <c r="I156" s="11" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="J156" t="s">
         <v>529</v>
@@ -10131,7 +10183,7 @@
         <v>1145</v>
       </c>
       <c r="I157" s="11" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="J157" t="s">
         <v>529</v>
@@ -10157,7 +10209,7 @@
         <v>1146</v>
       </c>
       <c r="I158" s="11" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="J158" t="s">
         <v>529</v>
@@ -10183,7 +10235,7 @@
         <v>1147</v>
       </c>
       <c r="I159" s="11" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="J159" t="s">
         <v>529</v>
@@ -10209,7 +10261,7 @@
         <v>1148</v>
       </c>
       <c r="I160" s="11" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="J160" t="s">
         <v>529</v>
@@ -10235,7 +10287,7 @@
         <v>1149</v>
       </c>
       <c r="I161" s="11" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="J161" t="s">
         <v>529</v>
@@ -10261,7 +10313,7 @@
         <v>1150</v>
       </c>
       <c r="I162" s="11" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="J162" t="s">
         <v>529</v>
@@ -10313,7 +10365,7 @@
         <v>1152</v>
       </c>
       <c r="I164" s="11" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="J164" t="s">
         <v>529</v>
@@ -10339,7 +10391,7 @@
         <v>1153</v>
       </c>
       <c r="I165" s="11" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="J165" t="s">
         <v>529</v>
@@ -10365,7 +10417,7 @@
         <v>1154</v>
       </c>
       <c r="I166" s="11" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="J166" t="s">
         <v>529</v>
@@ -10391,7 +10443,7 @@
         <v>1155</v>
       </c>
       <c r="I167" s="11" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="J167" t="s">
         <v>529</v>
@@ -10417,7 +10469,7 @@
         <v>1156</v>
       </c>
       <c r="I168" s="11" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="J168" t="s">
         <v>529</v>
@@ -10443,7 +10495,7 @@
         <v>1157</v>
       </c>
       <c r="I169" s="11" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="J169" t="s">
         <v>529</v>
@@ -10469,7 +10521,7 @@
         <v>1158</v>
       </c>
       <c r="I170" s="11" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="J170" t="s">
         <v>529</v>
@@ -10495,7 +10547,7 @@
         <v>1159</v>
       </c>
       <c r="I171" s="11" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="J171" t="s">
         <v>529</v>
@@ -10573,7 +10625,7 @@
         <v>1162</v>
       </c>
       <c r="I174" s="11" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="J174" t="s">
         <v>529</v>
@@ -10599,7 +10651,7 @@
         <v>1163</v>
       </c>
       <c r="I175" s="11" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="J175" t="s">
         <v>529</v>
@@ -10625,7 +10677,7 @@
         <v>1164</v>
       </c>
       <c r="I176" s="11" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="J176" t="s">
         <v>529</v>
@@ -10651,7 +10703,7 @@
         <v>1165</v>
       </c>
       <c r="I177" s="11" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="J177" t="s">
         <v>529</v>
@@ -10677,7 +10729,7 @@
         <v>1166</v>
       </c>
       <c r="I178" s="11" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="J178" t="s">
         <v>529</v>
@@ -10703,7 +10755,7 @@
         <v>1167</v>
       </c>
       <c r="I179" s="11" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="J179" t="s">
         <v>529</v>
@@ -10729,7 +10781,7 @@
         <v>1168</v>
       </c>
       <c r="I180" s="11" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="J180" t="s">
         <v>529</v>
@@ -10755,7 +10807,7 @@
         <v>1169</v>
       </c>
       <c r="I181" s="11" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="J181" t="s">
         <v>529</v>
@@ -10781,7 +10833,7 @@
         <v>1170</v>
       </c>
       <c r="I182" s="11" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="J182" t="s">
         <v>529</v>
@@ -10807,7 +10859,7 @@
         <v>1171</v>
       </c>
       <c r="I183" s="11" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="J183" t="s">
         <v>529</v>
@@ -10833,7 +10885,7 @@
         <v>1172</v>
       </c>
       <c r="I184" s="11" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="J184" t="s">
         <v>529</v>
@@ -10859,7 +10911,7 @@
         <v>1173</v>
       </c>
       <c r="I185" s="11" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="J185" t="s">
         <v>529</v>
@@ -10885,7 +10937,7 @@
         <v>1174</v>
       </c>
       <c r="I186" s="11" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="J186" t="s">
         <v>529</v>
@@ -10911,7 +10963,7 @@
         <v>1175</v>
       </c>
       <c r="I187" s="11" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="J187" t="s">
         <v>529</v>
@@ -10937,7 +10989,7 @@
         <v>1176</v>
       </c>
       <c r="I188" s="11" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="J188" t="s">
         <v>529</v>
@@ -10989,7 +11041,7 @@
         <v>1178</v>
       </c>
       <c r="I190" s="11" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="J190" t="s">
         <v>529</v>
@@ -11015,7 +11067,7 @@
         <v>1179</v>
       </c>
       <c r="I191" s="11" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="J191" t="s">
         <v>529</v>
@@ -11041,7 +11093,7 @@
         <v>1180</v>
       </c>
       <c r="I192" s="11" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="J192" t="s">
         <v>529</v>
@@ -11067,7 +11119,7 @@
         <v>1181</v>
       </c>
       <c r="I193" s="11" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="J193" t="s">
         <v>529</v>
@@ -11093,7 +11145,7 @@
         <v>1182</v>
       </c>
       <c r="I194" s="11" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="J194" t="s">
         <v>529</v>
@@ -11119,7 +11171,7 @@
         <v>1183</v>
       </c>
       <c r="I195" s="11" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J195" t="s">
         <v>529</v>
@@ -11145,7 +11197,7 @@
         <v>1184</v>
       </c>
       <c r="I196" s="11" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="J196" t="s">
         <v>529</v>
@@ -11171,7 +11223,7 @@
         <v>1185</v>
       </c>
       <c r="I197" s="11" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="J197" t="s">
         <v>529</v>
@@ -11197,7 +11249,7 @@
         <v>1186</v>
       </c>
       <c r="I198" s="11" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="J198" t="s">
         <v>529</v>
@@ -11223,7 +11275,7 @@
         <v>1187</v>
       </c>
       <c r="I199" s="11" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="J199" t="s">
         <v>529</v>
@@ -11249,7 +11301,7 @@
         <v>1188</v>
       </c>
       <c r="I200" s="11" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="J200" t="s">
         <v>529</v>
@@ -11275,7 +11327,7 @@
         <v>1189</v>
       </c>
       <c r="I201" s="11" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="J201" t="s">
         <v>529</v>
@@ -11301,7 +11353,7 @@
         <v>1190</v>
       </c>
       <c r="I202" s="11" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="J202" t="s">
         <v>529</v>
@@ -11327,7 +11379,7 @@
         <v>1191</v>
       </c>
       <c r="I203" s="11" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="J203" t="s">
         <v>529</v>
@@ -11353,7 +11405,7 @@
         <v>1192</v>
       </c>
       <c r="I204" s="11" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="J204" t="s">
         <v>529</v>
@@ -11379,7 +11431,7 @@
         <v>1193</v>
       </c>
       <c r="I205" s="11" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="J205" t="s">
         <v>529</v>
@@ -11405,7 +11457,7 @@
         <v>1194</v>
       </c>
       <c r="I206" s="11" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="J206" t="s">
         <v>529</v>
@@ -11431,7 +11483,7 @@
         <v>1195</v>
       </c>
       <c r="I207" s="11" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="J207" t="s">
         <v>529</v>
@@ -11457,7 +11509,7 @@
         <v>1196</v>
       </c>
       <c r="I208" s="11" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="J208" t="s">
         <v>529</v>
@@ -11483,7 +11535,7 @@
         <v>1197</v>
       </c>
       <c r="I209" s="11" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="J209" t="s">
         <v>529</v>
@@ -11509,7 +11561,7 @@
         <v>1198</v>
       </c>
       <c r="I210" s="11" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="J210" t="s">
         <v>529</v>
@@ -11535,7 +11587,7 @@
         <v>1199</v>
       </c>
       <c r="I211" s="11" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="J211" t="s">
         <v>529</v>
@@ -11561,7 +11613,7 @@
         <v>1200</v>
       </c>
       <c r="I212" s="11" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="J212" t="s">
         <v>529</v>
@@ -11587,7 +11639,7 @@
         <v>1201</v>
       </c>
       <c r="I213" s="11" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="J213" t="s">
         <v>529</v>
@@ -11613,7 +11665,7 @@
         <v>1202</v>
       </c>
       <c r="I214" s="11" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="J214" t="s">
         <v>529</v>
@@ -11665,7 +11717,7 @@
         <v>1204</v>
       </c>
       <c r="I216" s="11" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="J216" t="s">
         <v>529</v>
@@ -11691,7 +11743,7 @@
         <v>1205</v>
       </c>
       <c r="I217" s="11" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="J217" t="s">
         <v>529</v>
@@ -11717,7 +11769,7 @@
         <v>1206</v>
       </c>
       <c r="I218" s="11" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="J218" t="s">
         <v>529</v>
@@ -11743,7 +11795,7 @@
         <v>1207</v>
       </c>
       <c r="I219" s="11" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="J219" t="s">
         <v>529</v>
@@ -11769,7 +11821,7 @@
         <v>1208</v>
       </c>
       <c r="I220" s="11" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="J220" t="s">
         <v>529</v>
@@ -11795,7 +11847,7 @@
         <v>1209</v>
       </c>
       <c r="I221" s="11" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="J221" t="s">
         <v>529</v>
@@ -11821,7 +11873,7 @@
         <v>1210</v>
       </c>
       <c r="I222" s="11" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="J222" t="s">
         <v>529</v>
@@ -11847,7 +11899,7 @@
         <v>1211</v>
       </c>
       <c r="I223" s="11" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="J223" t="s">
         <v>529</v>
@@ -11873,7 +11925,7 @@
         <v>1212</v>
       </c>
       <c r="I224" s="11" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="J224" t="s">
         <v>529</v>
@@ -11899,7 +11951,7 @@
         <v>1213</v>
       </c>
       <c r="I225" s="11" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="J225" t="s">
         <v>529</v>
@@ -11925,7 +11977,7 @@
         <v>1214</v>
       </c>
       <c r="I226" s="11" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="J226" t="s">
         <v>529</v>
@@ -11951,7 +12003,7 @@
         <v>1215</v>
       </c>
       <c r="I227" s="11" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="J227" t="s">
         <v>529</v>
@@ -11977,7 +12029,7 @@
         <v>1216</v>
       </c>
       <c r="I228" s="11" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="J228" t="s">
         <v>529</v>
@@ -12003,7 +12055,7 @@
         <v>1217</v>
       </c>
       <c r="I229" s="11" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="J229" t="s">
         <v>529</v>
@@ -12029,7 +12081,7 @@
         <v>1218</v>
       </c>
       <c r="I230" s="11" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="J230" t="s">
         <v>529</v>
@@ -12055,7 +12107,7 @@
         <v>1219</v>
       </c>
       <c r="I231" s="11" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="J231" t="s">
         <v>529</v>
@@ -12081,7 +12133,7 @@
         <v>1220</v>
       </c>
       <c r="I232" s="11" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="J232" t="s">
         <v>529</v>
@@ -12107,7 +12159,7 @@
         <v>1221</v>
       </c>
       <c r="I233" s="11" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="J233" t="s">
         <v>529</v>
@@ -12133,7 +12185,7 @@
         <v>1222</v>
       </c>
       <c r="I234" s="11" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="J234" t="s">
         <v>529</v>
@@ -12159,7 +12211,7 @@
         <v>1223</v>
       </c>
       <c r="I235" s="11" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="J235" t="s">
         <v>529</v>
@@ -12185,7 +12237,7 @@
         <v>1112</v>
       </c>
       <c r="I236" s="11" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="J236" t="s">
         <v>529</v>
@@ -12211,7 +12263,7 @@
         <v>1224</v>
       </c>
       <c r="I237" s="11" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="J237" t="s">
         <v>528</v>
@@ -12237,7 +12289,7 @@
         <v>1225</v>
       </c>
       <c r="I238" s="11" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="J238" t="s">
         <v>528</v>
@@ -12289,7 +12341,7 @@
         <v>1227</v>
       </c>
       <c r="I240" s="11" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="J240" t="s">
         <v>528</v>
@@ -12315,7 +12367,7 @@
         <v>1228</v>
       </c>
       <c r="I241" s="11" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="J241" t="s">
         <v>528</v>
@@ -12341,7 +12393,7 @@
         <v>1229</v>
       </c>
       <c r="I242" s="11" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="J242" t="s">
         <v>528</v>
@@ -12367,7 +12419,7 @@
         <v>1230</v>
       </c>
       <c r="I243" s="11" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="J243" t="s">
         <v>528</v>
@@ -12393,7 +12445,7 @@
         <v>1231</v>
       </c>
       <c r="I244" s="11" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="J244" t="s">
         <v>528</v>
@@ -12445,7 +12497,7 @@
         <v>1233</v>
       </c>
       <c r="I246" s="11" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="J246" t="s">
         <v>528</v>
@@ -12471,7 +12523,7 @@
         <v>1234</v>
       </c>
       <c r="I247" s="11" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="J247" t="s">
         <v>528</v>
@@ -12549,7 +12601,7 @@
         <v>1237</v>
       </c>
       <c r="I250" s="11" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="J250" t="s">
         <v>528</v>
@@ -12575,7 +12627,7 @@
         <v>1238</v>
       </c>
       <c r="I251" s="11" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="J251" t="s">
         <v>528</v>
@@ -12601,7 +12653,7 @@
         <v>1239</v>
       </c>
       <c r="I252" s="11" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="J252" t="s">
         <v>528</v>
@@ -12627,7 +12679,7 @@
         <v>1240</v>
       </c>
       <c r="I253" s="11" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="J253" t="s">
         <v>528</v>
@@ -12653,7 +12705,7 @@
         <v>1241</v>
       </c>
       <c r="I254" s="11" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="J254" t="s">
         <v>528</v>
@@ -12679,7 +12731,7 @@
         <v>1242</v>
       </c>
       <c r="I255" s="11" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="J255" t="s">
         <v>528</v>
@@ -12705,7 +12757,7 @@
         <v>1243</v>
       </c>
       <c r="I256" s="11" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="J256" t="s">
         <v>528</v>
@@ -12731,7 +12783,7 @@
         <v>1244</v>
       </c>
       <c r="I257" s="11" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="J257" t="s">
         <v>528</v>
@@ -12757,7 +12809,7 @@
         <v>1245</v>
       </c>
       <c r="I258" s="11" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="J258" t="s">
         <v>528</v>
@@ -12783,7 +12835,7 @@
         <v>1246</v>
       </c>
       <c r="I259" s="11" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="J259" t="s">
         <v>528</v>
@@ -12809,7 +12861,7 @@
         <v>1247</v>
       </c>
       <c r="I260" s="11" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="J260" t="s">
         <v>528</v>
@@ -12835,7 +12887,7 @@
         <v>1248</v>
       </c>
       <c r="I261" s="11" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="J261" t="s">
         <v>528</v>
@@ -12861,7 +12913,7 @@
         <v>1249</v>
       </c>
       <c r="I262" s="11" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="J262" t="s">
         <v>528</v>
@@ -12887,7 +12939,7 @@
         <v>1250</v>
       </c>
       <c r="I263" s="11" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="J263" t="s">
         <v>528</v>
@@ -12913,7 +12965,7 @@
         <v>1251</v>
       </c>
       <c r="I264" s="11" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="J264" t="s">
         <v>528</v>
@@ -12939,7 +12991,7 @@
         <v>1252</v>
       </c>
       <c r="I265" s="11" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="J265" t="s">
         <v>528</v>
@@ -12965,7 +13017,7 @@
         <v>1253</v>
       </c>
       <c r="I266" s="11" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="J266" t="s">
         <v>528</v>
@@ -12991,7 +13043,7 @@
         <v>1254</v>
       </c>
       <c r="I267" s="11" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="J267" t="s">
         <v>528</v>
@@ -13017,7 +13069,7 @@
         <v>1255</v>
       </c>
       <c r="I268" s="11" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="J268" t="s">
         <v>528</v>
@@ -13043,7 +13095,7 @@
         <v>1256</v>
       </c>
       <c r="I269" s="11" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="J269" t="s">
         <v>528</v>
@@ -13069,7 +13121,7 @@
         <v>1257</v>
       </c>
       <c r="I270" s="11" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="J270" t="s">
         <v>528</v>
@@ -13095,7 +13147,7 @@
         <v>1258</v>
       </c>
       <c r="I271" s="11" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="J271" t="s">
         <v>528</v>
@@ -13121,7 +13173,7 @@
         <v>1259</v>
       </c>
       <c r="I272" s="11" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="J272" t="s">
         <v>528</v>
@@ -13147,7 +13199,7 @@
         <v>1260</v>
       </c>
       <c r="I273" s="11" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="J273" t="s">
         <v>528</v>
@@ -13173,7 +13225,7 @@
         <v>1261</v>
       </c>
       <c r="I274" s="11" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="J274" t="s">
         <v>528</v>
@@ -13199,7 +13251,7 @@
         <v>1262</v>
       </c>
       <c r="I275" s="11" t="s">
-        <v>1747</v>
+        <v>1884</v>
       </c>
       <c r="J275" t="s">
         <v>528</v>
@@ -13225,7 +13277,7 @@
         <v>1263</v>
       </c>
       <c r="I276" s="11" t="s">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="J276" t="s">
         <v>528</v>
@@ -13251,7 +13303,7 @@
         <v>1264</v>
       </c>
       <c r="I277" s="11" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
       <c r="J277" t="s">
         <v>528</v>
@@ -13277,7 +13329,7 @@
         <v>1265</v>
       </c>
       <c r="I278" s="11" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
       <c r="J278" t="s">
         <v>528</v>
@@ -13303,7 +13355,7 @@
         <v>1266</v>
       </c>
       <c r="I279" s="11" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
       <c r="J279" t="s">
         <v>528</v>
@@ -13329,7 +13381,7 @@
         <v>1267</v>
       </c>
       <c r="I280" s="11" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="J280" t="s">
         <v>528</v>
@@ -13355,7 +13407,7 @@
         <v>1268</v>
       </c>
       <c r="I281" s="11" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
       <c r="J281" t="s">
         <v>528</v>
@@ -13381,7 +13433,7 @@
         <v>1269</v>
       </c>
       <c r="I282" s="11" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
       <c r="J282" t="s">
         <v>528</v>
@@ -13407,7 +13459,7 @@
         <v>1270</v>
       </c>
       <c r="I283" s="11" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="J283" t="s">
         <v>528</v>
@@ -13433,7 +13485,7 @@
         <v>1271</v>
       </c>
       <c r="I284" s="11" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="J284" t="s">
         <v>528</v>
@@ -13459,7 +13511,7 @@
         <v>1272</v>
       </c>
       <c r="I285" s="11" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
       <c r="J285" t="s">
         <v>528</v>
@@ -13485,7 +13537,7 @@
         <v>1273</v>
       </c>
       <c r="I286" s="11" t="s">
-        <v>1758</v>
+        <v>1756</v>
       </c>
       <c r="J286" t="s">
         <v>528</v>
@@ -13511,7 +13563,7 @@
         <v>1274</v>
       </c>
       <c r="I287" s="11" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="J287" t="s">
         <v>528</v>
@@ -13537,7 +13589,7 @@
         <v>1275</v>
       </c>
       <c r="I288" s="11" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="J288" t="s">
         <v>528</v>
@@ -13589,7 +13641,7 @@
         <v>1277</v>
       </c>
       <c r="I290" s="11" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="J290" t="s">
         <v>530</v>
@@ -13615,7 +13667,7 @@
         <v>1278</v>
       </c>
       <c r="I291" s="11" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="J291" t="s">
         <v>530</v>
@@ -13641,7 +13693,7 @@
         <v>1279</v>
       </c>
       <c r="I292" s="11" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
       <c r="J292" t="s">
         <v>530</v>
@@ -13667,7 +13719,7 @@
         <v>1092</v>
       </c>
       <c r="I293" s="11" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="J293" t="s">
         <v>530</v>
@@ -13693,7 +13745,7 @@
         <v>1280</v>
       </c>
       <c r="I294" s="11" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="J294" t="s">
         <v>530</v>
@@ -13719,7 +13771,7 @@
         <v>1281</v>
       </c>
       <c r="I295" s="11" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
       <c r="J295" t="s">
         <v>530</v>
@@ -13745,7 +13797,7 @@
         <v>1282</v>
       </c>
       <c r="I296" s="11" t="s">
-        <v>1766</v>
+        <v>1764</v>
       </c>
       <c r="J296" t="s">
         <v>530</v>
@@ -13771,7 +13823,7 @@
         <v>1283</v>
       </c>
       <c r="I297" s="11" t="s">
-        <v>1767</v>
+        <v>1765</v>
       </c>
       <c r="J297" t="s">
         <v>530</v>
@@ -13797,7 +13849,7 @@
         <v>1284</v>
       </c>
       <c r="I298" s="11" t="s">
-        <v>1768</v>
+        <v>1766</v>
       </c>
       <c r="J298" t="s">
         <v>530</v>
@@ -13823,7 +13875,7 @@
         <v>1285</v>
       </c>
       <c r="I299" s="11" t="s">
-        <v>1769</v>
+        <v>1767</v>
       </c>
       <c r="J299" t="s">
         <v>530</v>
@@ -13849,7 +13901,7 @@
         <v>1286</v>
       </c>
       <c r="I300" s="11" t="s">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="J300" t="s">
         <v>530</v>
@@ -13875,7 +13927,7 @@
         <v>1287</v>
       </c>
       <c r="I301" s="11" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
       <c r="J301" t="s">
         <v>530</v>
@@ -13901,7 +13953,7 @@
         <v>1288</v>
       </c>
       <c r="I302" s="11" t="s">
-        <v>1772</v>
+        <v>1770</v>
       </c>
       <c r="J302" t="s">
         <v>530</v>
@@ -13927,7 +13979,7 @@
         <v>1289</v>
       </c>
       <c r="I303" s="11" t="s">
-        <v>1773</v>
+        <v>1771</v>
       </c>
       <c r="J303" t="s">
         <v>530</v>
@@ -13953,7 +14005,7 @@
         <v>1290</v>
       </c>
       <c r="I304" s="11" t="s">
-        <v>1774</v>
+        <v>1772</v>
       </c>
       <c r="J304" t="s">
         <v>530</v>
@@ -13979,7 +14031,7 @@
         <v>1291</v>
       </c>
       <c r="I305" s="11" t="s">
-        <v>1775</v>
+        <v>1773</v>
       </c>
       <c r="J305" t="s">
         <v>530</v>
@@ -14005,7 +14057,7 @@
         <v>1292</v>
       </c>
       <c r="I306" s="11" t="s">
-        <v>1776</v>
+        <v>1774</v>
       </c>
       <c r="J306" t="s">
         <v>530</v>
@@ -14031,7 +14083,7 @@
         <v>1213</v>
       </c>
       <c r="I307" s="11" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="J307" t="s">
         <v>530</v>
@@ -14057,7 +14109,7 @@
         <v>1293</v>
       </c>
       <c r="I308" s="11" t="s">
-        <v>1777</v>
+        <v>1775</v>
       </c>
       <c r="J308" t="s">
         <v>530</v>
@@ -14083,7 +14135,7 @@
         <v>1294</v>
       </c>
       <c r="I309" s="11" t="s">
-        <v>1778</v>
+        <v>1776</v>
       </c>
       <c r="J309" t="s">
         <v>530</v>
@@ -14109,7 +14161,7 @@
         <v>1295</v>
       </c>
       <c r="I310" s="11" t="s">
-        <v>1779</v>
+        <v>1777</v>
       </c>
       <c r="J310" t="s">
         <v>530</v>
@@ -14135,7 +14187,7 @@
         <v>1296</v>
       </c>
       <c r="I311" s="11" t="s">
-        <v>1780</v>
+        <v>1778</v>
       </c>
       <c r="J311" t="s">
         <v>530</v>
@@ -14161,7 +14213,7 @@
         <v>1297</v>
       </c>
       <c r="I312" s="11" t="s">
-        <v>1781</v>
+        <v>1779</v>
       </c>
       <c r="J312" t="s">
         <v>530</v>
@@ -14187,7 +14239,7 @@
         <v>1298</v>
       </c>
       <c r="I313" s="11" t="s">
-        <v>1782</v>
+        <v>1780</v>
       </c>
       <c r="J313" t="s">
         <v>530</v>
@@ -14213,7 +14265,7 @@
         <v>1084</v>
       </c>
       <c r="I314" s="11" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="J314" t="s">
         <v>530</v>
@@ -14239,7 +14291,7 @@
         <v>1299</v>
       </c>
       <c r="I315" s="11" t="s">
-        <v>1783</v>
+        <v>1781</v>
       </c>
       <c r="J315" t="s">
         <v>530</v>
@@ -14265,7 +14317,7 @@
         <v>1300</v>
       </c>
       <c r="I316" s="11" t="s">
-        <v>1784</v>
+        <v>1782</v>
       </c>
       <c r="J316" t="s">
         <v>530</v>
@@ -14291,7 +14343,7 @@
         <v>1301</v>
       </c>
       <c r="I317" s="11" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="J317" t="s">
         <v>530</v>
@@ -14317,7 +14369,7 @@
         <v>1302</v>
       </c>
       <c r="I318" s="11" t="s">
-        <v>1786</v>
+        <v>1784</v>
       </c>
       <c r="J318" t="s">
         <v>530</v>
@@ -14343,7 +14395,7 @@
         <v>1303</v>
       </c>
       <c r="I319" s="11" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="J319" t="s">
         <v>530</v>
@@ -14369,7 +14421,7 @@
         <v>1304</v>
       </c>
       <c r="I320" s="11" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
       <c r="J320" t="s">
         <v>530</v>
@@ -14421,7 +14473,7 @@
         <v>1306</v>
       </c>
       <c r="I322" s="11" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
       <c r="J322" t="s">
         <v>530</v>
@@ -14447,7 +14499,7 @@
         <v>1307</v>
       </c>
       <c r="I323" s="11" t="s">
-        <v>1790</v>
+        <v>1788</v>
       </c>
       <c r="J323" t="s">
         <v>530</v>
@@ -14473,7 +14525,7 @@
         <v>1308</v>
       </c>
       <c r="I324" s="11" t="s">
-        <v>1791</v>
+        <v>1789</v>
       </c>
       <c r="J324" t="s">
         <v>530</v>
@@ -14499,7 +14551,7 @@
         <v>1309</v>
       </c>
       <c r="I325" s="11" t="s">
-        <v>1792</v>
+        <v>1790</v>
       </c>
       <c r="J325" t="s">
         <v>530</v>
@@ -14525,7 +14577,7 @@
         <v>1310</v>
       </c>
       <c r="I326" s="11" t="s">
-        <v>1793</v>
+        <v>1791</v>
       </c>
       <c r="J326" t="s">
         <v>530</v>
@@ -14551,7 +14603,7 @@
         <v>1311</v>
       </c>
       <c r="I327" s="11" t="s">
-        <v>1794</v>
+        <v>1792</v>
       </c>
       <c r="J327" t="s">
         <v>530</v>
@@ -14603,7 +14655,7 @@
         <v>1313</v>
       </c>
       <c r="I329" s="11" t="s">
-        <v>1795</v>
+        <v>1793</v>
       </c>
       <c r="J329" t="s">
         <v>530</v>
@@ -14629,7 +14681,7 @@
         <v>1314</v>
       </c>
       <c r="I330" s="11" t="s">
-        <v>1796</v>
+        <v>1794</v>
       </c>
       <c r="J330" t="s">
         <v>530</v>
@@ -14655,7 +14707,7 @@
         <v>1315</v>
       </c>
       <c r="I331" s="11" t="s">
-        <v>1797</v>
+        <v>1795</v>
       </c>
       <c r="J331" t="s">
         <v>530</v>
@@ -14681,7 +14733,7 @@
         <v>1316</v>
       </c>
       <c r="I332" s="11" t="s">
-        <v>1798</v>
+        <v>1796</v>
       </c>
       <c r="J332" t="s">
         <v>530</v>
@@ -14707,7 +14759,7 @@
         <v>1317</v>
       </c>
       <c r="I333" s="11" t="s">
-        <v>1799</v>
+        <v>1797</v>
       </c>
       <c r="J333" t="s">
         <v>530</v>
@@ -14733,7 +14785,7 @@
         <v>1318</v>
       </c>
       <c r="I334" s="11" t="s">
-        <v>1800</v>
+        <v>1798</v>
       </c>
       <c r="J334" t="s">
         <v>530</v>
@@ -14759,7 +14811,7 @@
         <v>1319</v>
       </c>
       <c r="I335" s="11" t="s">
-        <v>1801</v>
+        <v>1799</v>
       </c>
       <c r="J335" t="s">
         <v>530</v>
@@ -14785,7 +14837,7 @@
         <v>1320</v>
       </c>
       <c r="I336" s="11" t="s">
-        <v>1802</v>
+        <v>1800</v>
       </c>
       <c r="J336" t="s">
         <v>530</v>
@@ -14811,7 +14863,7 @@
         <v>1321</v>
       </c>
       <c r="I337" s="11" t="s">
-        <v>1803</v>
+        <v>1801</v>
       </c>
       <c r="J337" t="s">
         <v>530</v>
@@ -14837,7 +14889,7 @@
         <v>1322</v>
       </c>
       <c r="I338" s="11" t="s">
-        <v>1804</v>
+        <v>1802</v>
       </c>
       <c r="J338" t="s">
         <v>530</v>
@@ -14863,7 +14915,7 @@
         <v>1323</v>
       </c>
       <c r="I339" s="11" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="J339" t="s">
         <v>530</v>
@@ -14889,7 +14941,7 @@
         <v>1324</v>
       </c>
       <c r="I340" s="11" t="s">
-        <v>1805</v>
+        <v>1803</v>
       </c>
       <c r="J340" t="s">
         <v>530</v>
@@ -14915,7 +14967,7 @@
         <v>1325</v>
       </c>
       <c r="I341" s="11" t="s">
-        <v>1806</v>
+        <v>1804</v>
       </c>
       <c r="J341" t="s">
         <v>530</v>
@@ -14941,7 +14993,7 @@
         <v>1326</v>
       </c>
       <c r="I342" s="11" t="s">
-        <v>1807</v>
+        <v>1805</v>
       </c>
       <c r="J342" t="s">
         <v>530</v>
@@ -14967,7 +15019,7 @@
         <v>1327</v>
       </c>
       <c r="I343" s="11" t="s">
-        <v>1808</v>
+        <v>1806</v>
       </c>
       <c r="J343" t="s">
         <v>530</v>
@@ -14993,7 +15045,7 @@
         <v>1328</v>
       </c>
       <c r="I344" s="11" t="s">
-        <v>1809</v>
+        <v>1807</v>
       </c>
       <c r="J344" t="s">
         <v>530</v>
@@ -15019,7 +15071,7 @@
         <v>1329</v>
       </c>
       <c r="I345" s="11" t="s">
-        <v>1810</v>
+        <v>1808</v>
       </c>
       <c r="J345" t="s">
         <v>530</v>
@@ -15045,7 +15097,7 @@
         <v>1330</v>
       </c>
       <c r="I346" s="11" t="s">
-        <v>1811</v>
+        <v>1809</v>
       </c>
       <c r="J346" t="s">
         <v>530</v>
@@ -15071,7 +15123,7 @@
         <v>1331</v>
       </c>
       <c r="I347" s="11" t="s">
-        <v>1812</v>
+        <v>1810</v>
       </c>
       <c r="J347" t="s">
         <v>530</v>
@@ -15097,7 +15149,7 @@
         <v>1332</v>
       </c>
       <c r="I348" s="11" t="s">
-        <v>1813</v>
+        <v>1811</v>
       </c>
       <c r="J348" t="s">
         <v>530</v>
@@ -15123,7 +15175,7 @@
         <v>1333</v>
       </c>
       <c r="I349" s="11" t="s">
-        <v>1814</v>
+        <v>1812</v>
       </c>
       <c r="J349" t="s">
         <v>530</v>
@@ -15149,7 +15201,7 @@
         <v>1334</v>
       </c>
       <c r="I350" s="11" t="s">
-        <v>1815</v>
+        <v>1813</v>
       </c>
       <c r="J350" t="s">
         <v>530</v>
@@ -15175,7 +15227,7 @@
         <v>1335</v>
       </c>
       <c r="I351" s="11" t="s">
-        <v>1816</v>
+        <v>1814</v>
       </c>
       <c r="J351" t="s">
         <v>530</v>
@@ -15201,7 +15253,7 @@
         <v>1336</v>
       </c>
       <c r="I352" s="11" t="s">
-        <v>1817</v>
+        <v>1815</v>
       </c>
       <c r="J352" t="s">
         <v>530</v>
@@ -15253,7 +15305,7 @@
         <v>1338</v>
       </c>
       <c r="I354" s="11" t="s">
-        <v>1818</v>
+        <v>1816</v>
       </c>
       <c r="J354" t="s">
         <v>530</v>
@@ -15279,7 +15331,7 @@
         <v>1339</v>
       </c>
       <c r="I355" s="11" t="s">
-        <v>1819</v>
+        <v>1817</v>
       </c>
       <c r="J355" t="s">
         <v>530</v>
@@ -15305,7 +15357,7 @@
         <v>1340</v>
       </c>
       <c r="I356" s="11" t="s">
-        <v>1820</v>
+        <v>1818</v>
       </c>
       <c r="J356" t="s">
         <v>530</v>
@@ -15331,7 +15383,7 @@
         <v>1341</v>
       </c>
       <c r="I357" s="11" t="s">
-        <v>1821</v>
+        <v>1819</v>
       </c>
       <c r="J357" t="s">
         <v>530</v>
@@ -15357,7 +15409,7 @@
         <v>1342</v>
       </c>
       <c r="I358" s="11" t="s">
-        <v>1822</v>
+        <v>1820</v>
       </c>
       <c r="J358" t="s">
         <v>530</v>
@@ -15383,7 +15435,7 @@
         <v>1343</v>
       </c>
       <c r="I359" s="11" t="s">
-        <v>1823</v>
+        <v>1821</v>
       </c>
       <c r="J359" t="s">
         <v>530</v>
@@ -15409,7 +15461,7 @@
         <v>1344</v>
       </c>
       <c r="I360" s="11" t="s">
-        <v>1824</v>
+        <v>1822</v>
       </c>
       <c r="J360" t="s">
         <v>530</v>
@@ -15435,7 +15487,7 @@
         <v>1345</v>
       </c>
       <c r="I361" s="11" t="s">
-        <v>1825</v>
+        <v>1823</v>
       </c>
       <c r="J361" t="s">
         <v>530</v>
@@ -15461,7 +15513,7 @@
         <v>1346</v>
       </c>
       <c r="I362" s="11" t="s">
-        <v>1826</v>
+        <v>1824</v>
       </c>
       <c r="J362" t="s">
         <v>530</v>
@@ -15487,7 +15539,7 @@
         <v>1347</v>
       </c>
       <c r="I363" s="11" t="s">
-        <v>1827</v>
+        <v>1825</v>
       </c>
       <c r="J363" t="s">
         <v>530</v>
@@ -15513,7 +15565,7 @@
         <v>1348</v>
       </c>
       <c r="I364" s="11" t="s">
-        <v>1828</v>
+        <v>1826</v>
       </c>
       <c r="J364" t="s">
         <v>530</v>
@@ -15539,7 +15591,7 @@
         <v>1349</v>
       </c>
       <c r="I365" s="11" t="s">
-        <v>1829</v>
+        <v>1827</v>
       </c>
       <c r="J365" t="s">
         <v>530</v>
@@ -15565,7 +15617,7 @@
         <v>1350</v>
       </c>
       <c r="I366" s="11" t="s">
-        <v>1830</v>
+        <v>1828</v>
       </c>
       <c r="J366" t="s">
         <v>530</v>
@@ -15591,7 +15643,7 @@
         <v>1351</v>
       </c>
       <c r="I367" s="11" t="s">
-        <v>1831</v>
+        <v>1829</v>
       </c>
       <c r="J367" t="s">
         <v>530</v>
@@ -15617,7 +15669,7 @@
         <v>1352</v>
       </c>
       <c r="I368" s="11" t="s">
-        <v>1832</v>
+        <v>1830</v>
       </c>
       <c r="J368" t="s">
         <v>530</v>
@@ -15643,7 +15695,7 @@
         <v>1353</v>
       </c>
       <c r="I369" s="11" t="s">
-        <v>1833</v>
+        <v>1831</v>
       </c>
       <c r="J369" t="s">
         <v>530</v>
@@ -15669,7 +15721,7 @@
         <v>1354</v>
       </c>
       <c r="I370" s="11" t="s">
-        <v>1834</v>
+        <v>1832</v>
       </c>
       <c r="J370" t="s">
         <v>530</v>
@@ -15695,7 +15747,7 @@
         <v>1355</v>
       </c>
       <c r="I371" s="11" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="J371" t="s">
         <v>530</v>
@@ -15721,7 +15773,7 @@
         <v>1356</v>
       </c>
       <c r="I372" s="11" t="s">
-        <v>1836</v>
+        <v>1834</v>
       </c>
       <c r="J372" t="s">
         <v>530</v>
@@ -15747,7 +15799,7 @@
         <v>1357</v>
       </c>
       <c r="I373" s="11" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
       <c r="J373" t="s">
         <v>530</v>
@@ -15773,7 +15825,7 @@
         <v>1358</v>
       </c>
       <c r="I374" s="11" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
       <c r="J374" t="s">
         <v>530</v>
@@ -15799,7 +15851,7 @@
         <v>1359</v>
       </c>
       <c r="I375" s="11" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="J375" t="s">
         <v>530</v>
@@ -15825,7 +15877,7 @@
         <v>1360</v>
       </c>
       <c r="I376" s="11" t="s">
-        <v>1840</v>
+        <v>1838</v>
       </c>
       <c r="J376" t="s">
         <v>530</v>
@@ -15851,7 +15903,7 @@
         <v>1361</v>
       </c>
       <c r="I377" s="11" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
       <c r="J377" t="s">
         <v>530</v>
@@ -15877,7 +15929,7 @@
         <v>1362</v>
       </c>
       <c r="I378" s="11" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="J378" t="s">
         <v>528</v>
@@ -15903,7 +15955,7 @@
         <v>1363</v>
       </c>
       <c r="I379" s="11" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
       <c r="J379" t="s">
         <v>528</v>
@@ -15929,7 +15981,7 @@
         <v>1364</v>
       </c>
       <c r="I380" s="11" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="J380" t="s">
         <v>528</v>
@@ -15955,7 +16007,7 @@
         <v>1365</v>
       </c>
       <c r="I381" s="11" t="s">
-        <v>1845</v>
+        <v>1843</v>
       </c>
       <c r="J381" t="s">
         <v>528</v>
@@ -15981,7 +16033,7 @@
         <v>1366</v>
       </c>
       <c r="I382" s="11" t="s">
-        <v>1846</v>
+        <v>1844</v>
       </c>
       <c r="J382" t="s">
         <v>528</v>
@@ -16007,7 +16059,7 @@
         <v>1367</v>
       </c>
       <c r="I383" s="11" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="J383" t="s">
         <v>528</v>
@@ -16033,7 +16085,7 @@
         <v>1368</v>
       </c>
       <c r="I384" s="11" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
       <c r="J384" t="s">
         <v>528</v>
@@ -16059,7 +16111,7 @@
         <v>1369</v>
       </c>
       <c r="I385" s="11" t="s">
-        <v>1849</v>
+        <v>1847</v>
       </c>
       <c r="J385" t="s">
         <v>528</v>
@@ -16085,7 +16137,7 @@
         <v>1370</v>
       </c>
       <c r="I386" s="11" t="s">
-        <v>1850</v>
+        <v>1848</v>
       </c>
       <c r="J386" t="s">
         <v>531</v>
@@ -16111,7 +16163,7 @@
         <v>1371</v>
       </c>
       <c r="I387" s="11" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="J387" t="s">
         <v>531</v>
@@ -16137,7 +16189,7 @@
         <v>1372</v>
       </c>
       <c r="I388" s="11" t="s">
-        <v>1852</v>
+        <v>1850</v>
       </c>
       <c r="J388" t="s">
         <v>531</v>
@@ -16163,7 +16215,7 @@
         <v>1373</v>
       </c>
       <c r="I389" s="11" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="J389" t="s">
         <v>531</v>
@@ -16189,7 +16241,7 @@
         <v>1374</v>
       </c>
       <c r="I390" s="11" t="s">
-        <v>1853</v>
+        <v>1851</v>
       </c>
       <c r="J390" t="s">
         <v>531</v>
@@ -16215,7 +16267,7 @@
         <v>1375</v>
       </c>
       <c r="I391" s="11" t="s">
-        <v>1854</v>
+        <v>1852</v>
       </c>
       <c r="J391" t="s">
         <v>531</v>
@@ -16241,7 +16293,7 @@
         <v>1376</v>
       </c>
       <c r="I392" s="11" t="s">
-        <v>1855</v>
+        <v>1853</v>
       </c>
       <c r="J392" t="s">
         <v>531</v>
@@ -16267,7 +16319,7 @@
         <v>1377</v>
       </c>
       <c r="I393" s="11" t="s">
-        <v>1856</v>
+        <v>1854</v>
       </c>
       <c r="J393" t="s">
         <v>531</v>
@@ -16293,7 +16345,7 @@
         <v>1378</v>
       </c>
       <c r="I394" s="11" t="s">
-        <v>1857</v>
+        <v>1855</v>
       </c>
       <c r="J394" t="s">
         <v>531</v>
@@ -16319,7 +16371,7 @@
         <v>1379</v>
       </c>
       <c r="I395" s="11" t="s">
-        <v>1858</v>
+        <v>1856</v>
       </c>
       <c r="J395" t="s">
         <v>531</v>
@@ -16345,7 +16397,7 @@
         <v>1380</v>
       </c>
       <c r="I396" s="11" t="s">
-        <v>1859</v>
+        <v>1857</v>
       </c>
       <c r="J396" t="s">
         <v>531</v>
@@ -16371,7 +16423,7 @@
         <v>1381</v>
       </c>
       <c r="I397" s="11" t="s">
-        <v>1860</v>
+        <v>1858</v>
       </c>
       <c r="J397" t="s">
         <v>531</v>
@@ -16397,7 +16449,7 @@
         <v>1382</v>
       </c>
       <c r="I398" s="11" t="s">
-        <v>1861</v>
+        <v>1859</v>
       </c>
       <c r="J398" t="s">
         <v>531</v>
@@ -16423,7 +16475,7 @@
         <v>1383</v>
       </c>
       <c r="I399" s="11" t="s">
-        <v>1862</v>
+        <v>1860</v>
       </c>
       <c r="J399" t="s">
         <v>531</v>
@@ -16449,7 +16501,7 @@
         <v>1384</v>
       </c>
       <c r="I400" s="11" t="s">
-        <v>1863</v>
+        <v>1861</v>
       </c>
       <c r="J400" t="s">
         <v>531</v>
@@ -16475,7 +16527,7 @@
         <v>1385</v>
       </c>
       <c r="I401" s="11" t="s">
-        <v>1864</v>
+        <v>1862</v>
       </c>
       <c r="J401" t="s">
         <v>531</v>
@@ -16501,7 +16553,7 @@
         <v>1386</v>
       </c>
       <c r="I402" s="11" t="s">
-        <v>1865</v>
+        <v>1863</v>
       </c>
       <c r="J402" t="s">
         <v>531</v>
@@ -16527,7 +16579,7 @@
         <v>1387</v>
       </c>
       <c r="I403" s="11" t="s">
-        <v>1866</v>
+        <v>1864</v>
       </c>
       <c r="J403" t="s">
         <v>531</v>
@@ -16553,7 +16605,7 @@
         <v>1388</v>
       </c>
       <c r="I404" s="11" t="s">
-        <v>1867</v>
+        <v>1865</v>
       </c>
       <c r="J404" t="s">
         <v>531</v>
@@ -16579,7 +16631,7 @@
         <v>1389</v>
       </c>
       <c r="I405" s="11" t="s">
-        <v>1808</v>
+        <v>1806</v>
       </c>
       <c r="J405" t="s">
         <v>531</v>
@@ -16605,7 +16657,7 @@
         <v>1390</v>
       </c>
       <c r="I406" s="11" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
       <c r="J406" t="s">
         <v>531</v>
@@ -16631,7 +16683,7 @@
         <v>1391</v>
       </c>
       <c r="I407" s="11" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="J407" t="s">
         <v>531</v>
@@ -16657,7 +16709,7 @@
         <v>1392</v>
       </c>
       <c r="I408" s="11" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="J408" t="s">
         <v>531</v>
@@ -16683,7 +16735,7 @@
         <v>1393</v>
       </c>
       <c r="I409" s="11" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="J409" t="s">
         <v>531</v>
@@ -16709,7 +16761,7 @@
         <v>1394</v>
       </c>
       <c r="I410" s="11" t="s">
-        <v>1870</v>
+        <v>1868</v>
       </c>
       <c r="J410" t="s">
         <v>531</v>
@@ -16735,7 +16787,7 @@
         <v>1395</v>
       </c>
       <c r="I411" s="11" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
       <c r="J411" t="s">
         <v>531</v>
@@ -16761,7 +16813,7 @@
         <v>1396</v>
       </c>
       <c r="I412" s="11" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
       <c r="J412" t="s">
         <v>531</v>
@@ -16787,7 +16839,7 @@
         <v>1397</v>
       </c>
       <c r="I413" s="11" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
       <c r="J413" t="s">
         <v>531</v>
@@ -16813,7 +16865,7 @@
         <v>1398</v>
       </c>
       <c r="I414" s="11" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
       <c r="J414" t="s">
         <v>531</v>
@@ -16839,7 +16891,7 @@
         <v>1399</v>
       </c>
       <c r="I415" s="11" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
       <c r="J415" t="s">
         <v>531</v>
@@ -16891,7 +16943,7 @@
         <v>1401</v>
       </c>
       <c r="I417" s="11" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="J417" t="s">
         <v>531</v>
@@ -16917,7 +16969,7 @@
         <v>1223</v>
       </c>
       <c r="I418" s="11" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="J418" t="s">
         <v>531</v>
@@ -16943,7 +16995,7 @@
         <v>1402</v>
       </c>
       <c r="I419" s="11" t="s">
-        <v>1874</v>
+        <v>1872</v>
       </c>
       <c r="J419" t="s">
         <v>531</v>
@@ -16969,7 +17021,7 @@
         <v>1403</v>
       </c>
       <c r="I420" s="11" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="J420" t="s">
         <v>531</v>
@@ -16995,7 +17047,7 @@
         <v>1264</v>
       </c>
       <c r="I421" s="11" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
       <c r="J421" t="s">
         <v>531</v>
@@ -17021,7 +17073,7 @@
         <v>1404</v>
       </c>
       <c r="I422" s="11" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
       <c r="J422" t="s">
         <v>531</v>
@@ -17047,7 +17099,7 @@
         <v>1405</v>
       </c>
       <c r="I423" s="11" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="J423" t="s">
         <v>531</v>
@@ -17073,7 +17125,7 @@
         <v>1406</v>
       </c>
       <c r="I424" s="11" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
       <c r="J424" t="s">
         <v>531</v>
@@ -17099,7 +17151,7 @@
         <v>1407</v>
       </c>
       <c r="I425" s="11" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="J425" t="s">
         <v>531</v>
@@ -17125,7 +17177,7 @@
         <v>1408</v>
       </c>
       <c r="I426" s="11" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
       <c r="J426" t="s">
         <v>531</v>
@@ -17151,7 +17203,7 @@
         <v>1409</v>
       </c>
       <c r="I427" s="11" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
       <c r="J427" t="s">
         <v>531</v>

</xml_diff>

<commit_message>
even more gloss fixes
</commit_message>
<xml_diff>
--- a/raw_data/Norwegian_WG/[Norwegian_WG].xlsx
+++ b/raw_data/Norwegian_WG/[Norwegian_WG].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3761" uniqueCount="1886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3761" uniqueCount="1888">
   <si>
     <t>item</t>
   </si>
@@ -4638,12 +4638,6 @@
     <t>meow</t>
   </si>
   <si>
-    <t>Need we say</t>
-  </si>
-  <si>
-    <t>tough-tough</t>
-  </si>
-  <si>
     <t>duck</t>
   </si>
   <si>
@@ -5289,9 +5283,6 @@
     <t>thank you</t>
   </si>
   <si>
-    <t>por favor</t>
-  </si>
-  <si>
     <t>hold it</t>
   </si>
   <si>
@@ -5310,9 +5301,6 @@
     <t>shove</t>
   </si>
   <si>
-    <t>making love</t>
-  </si>
-  <si>
     <t>get</t>
   </si>
   <si>
@@ -5677,6 +5665,24 @@
   </si>
   <si>
     <t>baa baa</t>
+  </si>
+  <si>
+    <t>moo</t>
+  </si>
+  <si>
+    <t>cockadoodledoo</t>
+  </si>
+  <si>
+    <t>ouch</t>
+  </si>
+  <si>
+    <t>choo choo</t>
+  </si>
+  <si>
+    <t>please</t>
+  </si>
+  <si>
+    <t>love</t>
   </si>
 </sst>
 </file>
@@ -5749,8 +5755,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5818,7 +5828,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -5840,6 +5850,8 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5861,6 +5873,8 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6192,8 +6206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="I296" sqref="I296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -6959,7 +6973,7 @@
         <v>1023</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>1536</v>
+        <v>1884</v>
       </c>
       <c r="J33" t="s">
         <v>528</v>
@@ -6985,7 +6999,7 @@
         <v>1024</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>1885</v>
+        <v>1881</v>
       </c>
       <c r="J34" t="s">
         <v>528</v>
@@ -7011,7 +7025,7 @@
         <v>1025</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>1881</v>
+        <v>1877</v>
       </c>
       <c r="J35" t="s">
         <v>528</v>
@@ -7037,7 +7051,7 @@
         <v>1026</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>1880</v>
+        <v>1876</v>
       </c>
       <c r="J36" t="s">
         <v>528</v>
@@ -7089,7 +7103,7 @@
         <v>1028</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>1028</v>
+        <v>1883</v>
       </c>
       <c r="J38" t="s">
         <v>528</v>
@@ -7141,7 +7155,7 @@
         <v>1030</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>1539</v>
+        <v>1882</v>
       </c>
       <c r="J40" t="s">
         <v>528</v>
@@ -7167,7 +7181,7 @@
         <v>1031</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>1883</v>
+        <v>1879</v>
       </c>
       <c r="J41" t="s">
         <v>528</v>
@@ -7193,7 +7207,7 @@
         <v>1032</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>1540</v>
+        <v>1885</v>
       </c>
       <c r="J42" t="s">
         <v>528</v>
@@ -7219,7 +7233,7 @@
         <v>1033</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>1882</v>
+        <v>1878</v>
       </c>
       <c r="J43" t="s">
         <v>528</v>
@@ -7245,7 +7259,7 @@
         <v>1034</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="J44" t="s">
         <v>529</v>
@@ -7271,7 +7285,7 @@
         <v>1035</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="J45" t="s">
         <v>529</v>
@@ -7297,7 +7311,7 @@
         <v>1036</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
       <c r="J46" t="s">
         <v>529</v>
@@ -7323,7 +7337,7 @@
         <v>1037</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="J47" t="s">
         <v>529</v>
@@ -7375,7 +7389,7 @@
         <v>1039</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="J49" t="s">
         <v>529</v>
@@ -7401,7 +7415,7 @@
         <v>1040</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="J50" t="s">
         <v>529</v>
@@ -7427,7 +7441,7 @@
         <v>1041</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
       <c r="J51" t="s">
         <v>529</v>
@@ -7453,7 +7467,7 @@
         <v>1042</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="J52" t="s">
         <v>529</v>
@@ -7505,7 +7519,7 @@
         <v>1044</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
       <c r="J54" t="s">
         <v>529</v>
@@ -7531,7 +7545,7 @@
         <v>1045</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="J55" t="s">
         <v>529</v>
@@ -7557,7 +7571,7 @@
         <v>1046</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="J56" t="s">
         <v>529</v>
@@ -7583,7 +7597,7 @@
         <v>1047</v>
       </c>
       <c r="I57" s="11" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="J57" t="s">
         <v>529</v>
@@ -7609,7 +7623,7 @@
         <v>1048</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="J58" t="s">
         <v>529</v>
@@ -7635,7 +7649,7 @@
         <v>1049</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
       <c r="J59" t="s">
         <v>529</v>
@@ -7661,7 +7675,7 @@
         <v>1050</v>
       </c>
       <c r="I60" s="11" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="J60" t="s">
         <v>529</v>
@@ -7687,7 +7701,7 @@
         <v>1051</v>
       </c>
       <c r="I61" s="11" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="J61" t="s">
         <v>529</v>
@@ -7713,7 +7727,7 @@
         <v>1052</v>
       </c>
       <c r="I62" s="11" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
       <c r="J62" t="s">
         <v>529</v>
@@ -7739,7 +7753,7 @@
         <v>1053</v>
       </c>
       <c r="I63" s="11" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="J63" t="s">
         <v>529</v>
@@ -7765,7 +7779,7 @@
         <v>1054</v>
       </c>
       <c r="I64" s="11" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="J64" t="s">
         <v>529</v>
@@ -7791,7 +7805,7 @@
         <v>1055</v>
       </c>
       <c r="I65" s="11" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="J65" t="s">
         <v>529</v>
@@ -7817,7 +7831,7 @@
         <v>1056</v>
       </c>
       <c r="I66" s="11" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
       <c r="J66" t="s">
         <v>529</v>
@@ -7843,7 +7857,7 @@
         <v>1057</v>
       </c>
       <c r="I67" s="11" t="s">
-        <v>1562</v>
+        <v>1560</v>
       </c>
       <c r="J67" t="s">
         <v>529</v>
@@ -7869,7 +7883,7 @@
         <v>1058</v>
       </c>
       <c r="I68" s="11" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
       <c r="J68" t="s">
         <v>529</v>
@@ -7895,7 +7909,7 @@
         <v>1059</v>
       </c>
       <c r="I69" s="11" t="s">
-        <v>1564</v>
+        <v>1562</v>
       </c>
       <c r="J69" t="s">
         <v>529</v>
@@ -7921,7 +7935,7 @@
         <v>1060</v>
       </c>
       <c r="I70" s="11" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
       <c r="J70" t="s">
         <v>529</v>
@@ -7947,7 +7961,7 @@
         <v>1061</v>
       </c>
       <c r="I71" s="11" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="J71" t="s">
         <v>529</v>
@@ -7999,7 +8013,7 @@
         <v>1063</v>
       </c>
       <c r="I73" s="11" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="J73" t="s">
         <v>529</v>
@@ -8025,7 +8039,7 @@
         <v>1064</v>
       </c>
       <c r="I74" s="11" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="J74" t="s">
         <v>529</v>
@@ -8051,7 +8065,7 @@
         <v>1065</v>
       </c>
       <c r="I75" s="11" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="J75" t="s">
         <v>529</v>
@@ -8103,7 +8117,7 @@
         <v>1067</v>
       </c>
       <c r="I77" s="11" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="J77" t="s">
         <v>529</v>
@@ -8129,7 +8143,7 @@
         <v>1068</v>
       </c>
       <c r="I78" s="11" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="J78" t="s">
         <v>529</v>
@@ -8155,7 +8169,7 @@
         <v>1069</v>
       </c>
       <c r="I79" s="11" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="J79" t="s">
         <v>529</v>
@@ -8181,7 +8195,7 @@
         <v>1070</v>
       </c>
       <c r="I80" s="11" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="J80" t="s">
         <v>529</v>
@@ -8207,7 +8221,7 @@
         <v>1071</v>
       </c>
       <c r="I81" s="11" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="J81" t="s">
         <v>529</v>
@@ -8233,7 +8247,7 @@
         <v>1072</v>
       </c>
       <c r="I82" s="11" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="J82" t="s">
         <v>529</v>
@@ -8259,7 +8273,7 @@
         <v>1073</v>
       </c>
       <c r="I83" s="11" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="J83" t="s">
         <v>529</v>
@@ -8285,7 +8299,7 @@
         <v>1074</v>
       </c>
       <c r="I84" s="11" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
       <c r="J84" t="s">
         <v>529</v>
@@ -8311,7 +8325,7 @@
         <v>1075</v>
       </c>
       <c r="I85" s="11" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="J85" t="s">
         <v>529</v>
@@ -8337,7 +8351,7 @@
         <v>1076</v>
       </c>
       <c r="I86" s="11" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="J86" t="s">
         <v>529</v>
@@ -8363,7 +8377,7 @@
         <v>1077</v>
       </c>
       <c r="I87" s="11" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="J87" t="s">
         <v>529</v>
@@ -8389,7 +8403,7 @@
         <v>1078</v>
       </c>
       <c r="I88" s="11" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="J88" t="s">
         <v>529</v>
@@ -8415,7 +8429,7 @@
         <v>1079</v>
       </c>
       <c r="I89" s="11" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="J89" t="s">
         <v>529</v>
@@ -8441,7 +8455,7 @@
         <v>1080</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="J90" t="s">
         <v>529</v>
@@ -8467,7 +8481,7 @@
         <v>1081</v>
       </c>
       <c r="I91" s="11" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="J91" t="s">
         <v>529</v>
@@ -8493,7 +8507,7 @@
         <v>1082</v>
       </c>
       <c r="I92" s="11" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="J92" t="s">
         <v>529</v>
@@ -8519,7 +8533,7 @@
         <v>1083</v>
       </c>
       <c r="I93" s="11" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="J93" t="s">
         <v>529</v>
@@ -8545,7 +8559,7 @@
         <v>1084</v>
       </c>
       <c r="I94" s="11" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="J94" t="s">
         <v>529</v>
@@ -8571,7 +8585,7 @@
         <v>1085</v>
       </c>
       <c r="I95" s="11" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="J95" t="s">
         <v>529</v>
@@ -8597,7 +8611,7 @@
         <v>1086</v>
       </c>
       <c r="I96" s="11" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="J96" t="s">
         <v>529</v>
@@ -8623,7 +8637,7 @@
         <v>1087</v>
       </c>
       <c r="I97" s="11" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="J97" t="s">
         <v>529</v>
@@ -8649,7 +8663,7 @@
         <v>1088</v>
       </c>
       <c r="I98" s="11" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="J98" t="s">
         <v>529</v>
@@ -8675,7 +8689,7 @@
         <v>1089</v>
       </c>
       <c r="I99" s="11" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="J99" t="s">
         <v>529</v>
@@ -8701,7 +8715,7 @@
         <v>1090</v>
       </c>
       <c r="I100" s="11" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
       <c r="J100" t="s">
         <v>529</v>
@@ -8753,7 +8767,7 @@
         <v>1092</v>
       </c>
       <c r="I102" s="11" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="J102" t="s">
         <v>529</v>
@@ -8779,7 +8793,7 @@
         <v>1093</v>
       </c>
       <c r="I103" s="11" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="J103" t="s">
         <v>529</v>
@@ -8805,7 +8819,7 @@
         <v>1094</v>
       </c>
       <c r="I104" s="11" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
       <c r="J104" t="s">
         <v>529</v>
@@ -8831,7 +8845,7 @@
         <v>1042</v>
       </c>
       <c r="I105" s="11" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="J105" t="s">
         <v>529</v>
@@ -8857,7 +8871,7 @@
         <v>1095</v>
       </c>
       <c r="I106" s="11" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
       <c r="J106" t="s">
         <v>529</v>
@@ -8883,7 +8897,7 @@
         <v>1096</v>
       </c>
       <c r="I107" s="11" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="J107" t="s">
         <v>529</v>
@@ -8909,7 +8923,7 @@
         <v>1097</v>
       </c>
       <c r="I108" s="11" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="J108" t="s">
         <v>529</v>
@@ -8961,7 +8975,7 @@
         <v>1099</v>
       </c>
       <c r="I110" s="11" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="J110" t="s">
         <v>529</v>
@@ -8987,7 +9001,7 @@
         <v>1100</v>
       </c>
       <c r="I111" s="11" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
       <c r="J111" t="s">
         <v>529</v>
@@ -9013,7 +9027,7 @@
         <v>1101</v>
       </c>
       <c r="I112" s="11" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="J112" t="s">
         <v>529</v>
@@ -9039,7 +9053,7 @@
         <v>1102</v>
       </c>
       <c r="I113" s="11" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="J113" t="s">
         <v>529</v>
@@ -9065,7 +9079,7 @@
         <v>1054</v>
       </c>
       <c r="I114" s="11" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
       <c r="J114" t="s">
         <v>529</v>
@@ -9091,7 +9105,7 @@
         <v>1103</v>
       </c>
       <c r="I115" s="11" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="J115" t="s">
         <v>529</v>
@@ -9117,7 +9131,7 @@
         <v>1104</v>
       </c>
       <c r="I116" s="11" t="s">
-        <v>1605</v>
+        <v>1603</v>
       </c>
       <c r="J116" t="s">
         <v>529</v>
@@ -9143,7 +9157,7 @@
         <v>1105</v>
       </c>
       <c r="I117" s="11" t="s">
-        <v>1606</v>
+        <v>1604</v>
       </c>
       <c r="J117" t="s">
         <v>529</v>
@@ -9221,7 +9235,7 @@
         <v>1108</v>
       </c>
       <c r="I120" s="11" t="s">
-        <v>1607</v>
+        <v>1605</v>
       </c>
       <c r="J120" t="s">
         <v>529</v>
@@ -9247,7 +9261,7 @@
         <v>1109</v>
       </c>
       <c r="I121" s="11" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="J121" t="s">
         <v>529</v>
@@ -9273,7 +9287,7 @@
         <v>1110</v>
       </c>
       <c r="I122" s="11" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
       <c r="J122" t="s">
         <v>529</v>
@@ -9299,7 +9313,7 @@
         <v>1111</v>
       </c>
       <c r="I123" s="11" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="J123" t="s">
         <v>529</v>
@@ -9325,7 +9339,7 @@
         <v>1112</v>
       </c>
       <c r="I124" s="11" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="J124" t="s">
         <v>529</v>
@@ -9351,7 +9365,7 @@
         <v>1113</v>
       </c>
       <c r="I125" s="11" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="J125" t="s">
         <v>529</v>
@@ -9377,7 +9391,7 @@
         <v>1114</v>
       </c>
       <c r="I126" s="11" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
       <c r="J126" t="s">
         <v>529</v>
@@ -9403,7 +9417,7 @@
         <v>1115</v>
       </c>
       <c r="I127" s="11" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="J127" t="s">
         <v>529</v>
@@ -9429,7 +9443,7 @@
         <v>1116</v>
       </c>
       <c r="I128" s="11" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="J128" t="s">
         <v>529</v>
@@ -9455,7 +9469,7 @@
         <v>1117</v>
       </c>
       <c r="I129" s="11" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="J129" t="s">
         <v>529</v>
@@ -9481,7 +9495,7 @@
         <v>1118</v>
       </c>
       <c r="I130" s="11" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
       <c r="J130" t="s">
         <v>529</v>
@@ -9507,7 +9521,7 @@
         <v>1119</v>
       </c>
       <c r="I131" s="11" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="J131" t="s">
         <v>529</v>
@@ -9533,7 +9547,7 @@
         <v>1120</v>
       </c>
       <c r="I132" s="11" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="J132" t="s">
         <v>529</v>
@@ -9559,7 +9573,7 @@
         <v>1121</v>
       </c>
       <c r="I133" s="11" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
       <c r="J133" t="s">
         <v>529</v>
@@ -9585,7 +9599,7 @@
         <v>1122</v>
       </c>
       <c r="I134" s="11" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
       <c r="J134" t="s">
         <v>529</v>
@@ -9611,7 +9625,7 @@
         <v>1123</v>
       </c>
       <c r="I135" s="11" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
       <c r="J135" t="s">
         <v>529</v>
@@ -9663,7 +9677,7 @@
         <v>1125</v>
       </c>
       <c r="I137" s="11" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="J137" t="s">
         <v>529</v>
@@ -9689,7 +9703,7 @@
         <v>1126</v>
       </c>
       <c r="I138" s="11" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="J138" t="s">
         <v>529</v>
@@ -9715,7 +9729,7 @@
         <v>1127</v>
       </c>
       <c r="I139" s="11" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
       <c r="J139" t="s">
         <v>529</v>
@@ -9741,7 +9755,7 @@
         <v>1128</v>
       </c>
       <c r="I140" s="11" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="J140" t="s">
         <v>529</v>
@@ -9767,7 +9781,7 @@
         <v>1129</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="J141" t="s">
         <v>529</v>
@@ -9793,7 +9807,7 @@
         <v>1130</v>
       </c>
       <c r="I142" s="11" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="J142" t="s">
         <v>529</v>
@@ -9819,7 +9833,7 @@
         <v>1131</v>
       </c>
       <c r="I143" s="11" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
       <c r="J143" t="s">
         <v>529</v>
@@ -9845,7 +9859,7 @@
         <v>1132</v>
       </c>
       <c r="I144" s="11" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="J144" t="s">
         <v>529</v>
@@ -9871,7 +9885,7 @@
         <v>1133</v>
       </c>
       <c r="I145" s="11" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="J145" t="s">
         <v>529</v>
@@ -9923,7 +9937,7 @@
         <v>1135</v>
       </c>
       <c r="I147" s="11" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="J147" t="s">
         <v>529</v>
@@ -9975,7 +9989,7 @@
         <v>1137</v>
       </c>
       <c r="I149" s="11" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
       <c r="J149" t="s">
         <v>529</v>
@@ -10001,7 +10015,7 @@
         <v>1138</v>
       </c>
       <c r="I150" s="11" t="s">
-        <v>1634</v>
+        <v>1632</v>
       </c>
       <c r="J150" t="s">
         <v>529</v>
@@ -10027,7 +10041,7 @@
         <v>1139</v>
       </c>
       <c r="I151" s="11" t="s">
-        <v>1635</v>
+        <v>1633</v>
       </c>
       <c r="J151" t="s">
         <v>529</v>
@@ -10053,7 +10067,7 @@
         <v>1140</v>
       </c>
       <c r="I152" s="11" t="s">
-        <v>1636</v>
+        <v>1634</v>
       </c>
       <c r="J152" t="s">
         <v>529</v>
@@ -10079,7 +10093,7 @@
         <v>1141</v>
       </c>
       <c r="I153" s="11" t="s">
-        <v>1637</v>
+        <v>1635</v>
       </c>
       <c r="J153" t="s">
         <v>529</v>
@@ -10105,7 +10119,7 @@
         <v>1142</v>
       </c>
       <c r="I154" s="11" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="J154" t="s">
         <v>529</v>
@@ -10131,7 +10145,7 @@
         <v>1143</v>
       </c>
       <c r="I155" s="11" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
       <c r="J155" t="s">
         <v>529</v>
@@ -10157,7 +10171,7 @@
         <v>1144</v>
       </c>
       <c r="I156" s="11" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="J156" t="s">
         <v>529</v>
@@ -10183,7 +10197,7 @@
         <v>1145</v>
       </c>
       <c r="I157" s="11" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="J157" t="s">
         <v>529</v>
@@ -10209,7 +10223,7 @@
         <v>1146</v>
       </c>
       <c r="I158" s="11" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="J158" t="s">
         <v>529</v>
@@ -10235,7 +10249,7 @@
         <v>1147</v>
       </c>
       <c r="I159" s="11" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
       <c r="J159" t="s">
         <v>529</v>
@@ -10261,7 +10275,7 @@
         <v>1148</v>
       </c>
       <c r="I160" s="11" t="s">
-        <v>1644</v>
+        <v>1642</v>
       </c>
       <c r="J160" t="s">
         <v>529</v>
@@ -10287,7 +10301,7 @@
         <v>1149</v>
       </c>
       <c r="I161" s="11" t="s">
-        <v>1645</v>
+        <v>1643</v>
       </c>
       <c r="J161" t="s">
         <v>529</v>
@@ -10313,7 +10327,7 @@
         <v>1150</v>
       </c>
       <c r="I162" s="11" t="s">
-        <v>1646</v>
+        <v>1644</v>
       </c>
       <c r="J162" t="s">
         <v>529</v>
@@ -10365,7 +10379,7 @@
         <v>1152</v>
       </c>
       <c r="I164" s="11" t="s">
-        <v>1647</v>
+        <v>1645</v>
       </c>
       <c r="J164" t="s">
         <v>529</v>
@@ -10391,7 +10405,7 @@
         <v>1153</v>
       </c>
       <c r="I165" s="11" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
       <c r="J165" t="s">
         <v>529</v>
@@ -10417,7 +10431,7 @@
         <v>1154</v>
       </c>
       <c r="I166" s="11" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
       <c r="J166" t="s">
         <v>529</v>
@@ -10443,7 +10457,7 @@
         <v>1155</v>
       </c>
       <c r="I167" s="11" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="J167" t="s">
         <v>529</v>
@@ -10469,7 +10483,7 @@
         <v>1156</v>
       </c>
       <c r="I168" s="11" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="J168" t="s">
         <v>529</v>
@@ -10495,7 +10509,7 @@
         <v>1157</v>
       </c>
       <c r="I169" s="11" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
       <c r="J169" t="s">
         <v>529</v>
@@ -10521,7 +10535,7 @@
         <v>1158</v>
       </c>
       <c r="I170" s="11" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
       <c r="J170" t="s">
         <v>529</v>
@@ -10547,7 +10561,7 @@
         <v>1159</v>
       </c>
       <c r="I171" s="11" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="J171" t="s">
         <v>529</v>
@@ -10625,7 +10639,7 @@
         <v>1162</v>
       </c>
       <c r="I174" s="11" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="J174" t="s">
         <v>529</v>
@@ -10651,7 +10665,7 @@
         <v>1163</v>
       </c>
       <c r="I175" s="11" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
       <c r="J175" t="s">
         <v>529</v>
@@ -10677,7 +10691,7 @@
         <v>1164</v>
       </c>
       <c r="I176" s="11" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
       <c r="J176" t="s">
         <v>529</v>
@@ -10703,7 +10717,7 @@
         <v>1165</v>
       </c>
       <c r="I177" s="11" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="J177" t="s">
         <v>529</v>
@@ -10729,7 +10743,7 @@
         <v>1166</v>
       </c>
       <c r="I178" s="11" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="J178" t="s">
         <v>529</v>
@@ -10755,7 +10769,7 @@
         <v>1167</v>
       </c>
       <c r="I179" s="11" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="J179" t="s">
         <v>529</v>
@@ -10781,7 +10795,7 @@
         <v>1168</v>
       </c>
       <c r="I180" s="11" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
       <c r="J180" t="s">
         <v>529</v>
@@ -10807,7 +10821,7 @@
         <v>1169</v>
       </c>
       <c r="I181" s="11" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
       <c r="J181" t="s">
         <v>529</v>
@@ -10833,7 +10847,7 @@
         <v>1170</v>
       </c>
       <c r="I182" s="11" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
       <c r="J182" t="s">
         <v>529</v>
@@ -10859,7 +10873,7 @@
         <v>1171</v>
       </c>
       <c r="I183" s="11" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="J183" t="s">
         <v>529</v>
@@ -10885,7 +10899,7 @@
         <v>1172</v>
       </c>
       <c r="I184" s="11" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="J184" t="s">
         <v>529</v>
@@ -10911,7 +10925,7 @@
         <v>1173</v>
       </c>
       <c r="I185" s="11" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
       <c r="J185" t="s">
         <v>529</v>
@@ -10937,7 +10951,7 @@
         <v>1174</v>
       </c>
       <c r="I186" s="11" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
       <c r="J186" t="s">
         <v>529</v>
@@ -10963,7 +10977,7 @@
         <v>1175</v>
       </c>
       <c r="I187" s="11" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="J187" t="s">
         <v>529</v>
@@ -10989,7 +11003,7 @@
         <v>1176</v>
       </c>
       <c r="I188" s="11" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
       <c r="J188" t="s">
         <v>529</v>
@@ -11041,7 +11055,7 @@
         <v>1178</v>
       </c>
       <c r="I190" s="11" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
       <c r="J190" t="s">
         <v>529</v>
@@ -11067,7 +11081,7 @@
         <v>1179</v>
       </c>
       <c r="I191" s="11" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="J191" t="s">
         <v>529</v>
@@ -11093,7 +11107,7 @@
         <v>1180</v>
       </c>
       <c r="I192" s="11" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="J192" t="s">
         <v>529</v>
@@ -11119,7 +11133,7 @@
         <v>1181</v>
       </c>
       <c r="I193" s="11" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
       <c r="J193" t="s">
         <v>529</v>
@@ -11145,7 +11159,7 @@
         <v>1182</v>
       </c>
       <c r="I194" s="11" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="J194" t="s">
         <v>529</v>
@@ -11171,7 +11185,7 @@
         <v>1183</v>
       </c>
       <c r="I195" s="11" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
       <c r="J195" t="s">
         <v>529</v>
@@ -11197,7 +11211,7 @@
         <v>1184</v>
       </c>
       <c r="I196" s="11" t="s">
-        <v>1676</v>
+        <v>1674</v>
       </c>
       <c r="J196" t="s">
         <v>529</v>
@@ -11223,7 +11237,7 @@
         <v>1185</v>
       </c>
       <c r="I197" s="11" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
       <c r="J197" t="s">
         <v>529</v>
@@ -11249,7 +11263,7 @@
         <v>1186</v>
       </c>
       <c r="I198" s="11" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="J198" t="s">
         <v>529</v>
@@ -11275,7 +11289,7 @@
         <v>1187</v>
       </c>
       <c r="I199" s="11" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="J199" t="s">
         <v>529</v>
@@ -11301,7 +11315,7 @@
         <v>1188</v>
       </c>
       <c r="I200" s="11" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="J200" t="s">
         <v>529</v>
@@ -11327,7 +11341,7 @@
         <v>1189</v>
       </c>
       <c r="I201" s="11" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="J201" t="s">
         <v>529</v>
@@ -11353,7 +11367,7 @@
         <v>1190</v>
       </c>
       <c r="I202" s="11" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
       <c r="J202" t="s">
         <v>529</v>
@@ -11379,7 +11393,7 @@
         <v>1191</v>
       </c>
       <c r="I203" s="11" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="J203" t="s">
         <v>529</v>
@@ -11405,7 +11419,7 @@
         <v>1192</v>
       </c>
       <c r="I204" s="11" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="J204" t="s">
         <v>529</v>
@@ -11431,7 +11445,7 @@
         <v>1193</v>
       </c>
       <c r="I205" s="11" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="J205" t="s">
         <v>529</v>
@@ -11457,7 +11471,7 @@
         <v>1194</v>
       </c>
       <c r="I206" s="11" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="J206" t="s">
         <v>529</v>
@@ -11483,7 +11497,7 @@
         <v>1195</v>
       </c>
       <c r="I207" s="11" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="J207" t="s">
         <v>529</v>
@@ -11509,7 +11523,7 @@
         <v>1196</v>
       </c>
       <c r="I208" s="11" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="J208" t="s">
         <v>529</v>
@@ -11535,7 +11549,7 @@
         <v>1197</v>
       </c>
       <c r="I209" s="11" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
       <c r="J209" t="s">
         <v>529</v>
@@ -11561,7 +11575,7 @@
         <v>1198</v>
       </c>
       <c r="I210" s="11" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="J210" t="s">
         <v>529</v>
@@ -11587,7 +11601,7 @@
         <v>1199</v>
       </c>
       <c r="I211" s="11" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="J211" t="s">
         <v>529</v>
@@ -11613,7 +11627,7 @@
         <v>1200</v>
       </c>
       <c r="I212" s="11" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="J212" t="s">
         <v>529</v>
@@ -11639,7 +11653,7 @@
         <v>1201</v>
       </c>
       <c r="I213" s="11" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="J213" t="s">
         <v>529</v>
@@ -11665,7 +11679,7 @@
         <v>1202</v>
       </c>
       <c r="I214" s="11" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
       <c r="J214" t="s">
         <v>529</v>
@@ -11717,7 +11731,7 @@
         <v>1204</v>
       </c>
       <c r="I216" s="11" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
       <c r="J216" t="s">
         <v>529</v>
@@ -11743,7 +11757,7 @@
         <v>1205</v>
       </c>
       <c r="I217" s="11" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
       <c r="J217" t="s">
         <v>529</v>
@@ -11769,7 +11783,7 @@
         <v>1206</v>
       </c>
       <c r="I218" s="11" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
       <c r="J218" t="s">
         <v>529</v>
@@ -11795,7 +11809,7 @@
         <v>1207</v>
       </c>
       <c r="I219" s="11" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="J219" t="s">
         <v>529</v>
@@ -11821,7 +11835,7 @@
         <v>1208</v>
       </c>
       <c r="I220" s="11" t="s">
-        <v>1699</v>
+        <v>1697</v>
       </c>
       <c r="J220" t="s">
         <v>529</v>
@@ -11847,7 +11861,7 @@
         <v>1209</v>
       </c>
       <c r="I221" s="11" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="J221" t="s">
         <v>529</v>
@@ -11873,7 +11887,7 @@
         <v>1210</v>
       </c>
       <c r="I222" s="11" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
       <c r="J222" t="s">
         <v>529</v>
@@ -11899,7 +11913,7 @@
         <v>1211</v>
       </c>
       <c r="I223" s="11" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
       <c r="J223" t="s">
         <v>529</v>
@@ -11925,7 +11939,7 @@
         <v>1212</v>
       </c>
       <c r="I224" s="11" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="J224" t="s">
         <v>529</v>
@@ -11951,7 +11965,7 @@
         <v>1213</v>
       </c>
       <c r="I225" s="11" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="J225" t="s">
         <v>529</v>
@@ -11977,7 +11991,7 @@
         <v>1214</v>
       </c>
       <c r="I226" s="11" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="J226" t="s">
         <v>529</v>
@@ -12003,7 +12017,7 @@
         <v>1215</v>
       </c>
       <c r="I227" s="11" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="J227" t="s">
         <v>529</v>
@@ -12029,7 +12043,7 @@
         <v>1216</v>
       </c>
       <c r="I228" s="11" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="J228" t="s">
         <v>529</v>
@@ -12055,7 +12069,7 @@
         <v>1217</v>
       </c>
       <c r="I229" s="11" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
       <c r="J229" t="s">
         <v>529</v>
@@ -12081,7 +12095,7 @@
         <v>1218</v>
       </c>
       <c r="I230" s="11" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="J230" t="s">
         <v>529</v>
@@ -12107,7 +12121,7 @@
         <v>1219</v>
       </c>
       <c r="I231" s="11" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="J231" t="s">
         <v>529</v>
@@ -12133,7 +12147,7 @@
         <v>1220</v>
       </c>
       <c r="I232" s="11" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="J232" t="s">
         <v>529</v>
@@ -12159,7 +12173,7 @@
         <v>1221</v>
       </c>
       <c r="I233" s="11" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="J233" t="s">
         <v>529</v>
@@ -12185,7 +12199,7 @@
         <v>1222</v>
       </c>
       <c r="I234" s="11" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="J234" t="s">
         <v>529</v>
@@ -12211,7 +12225,7 @@
         <v>1223</v>
       </c>
       <c r="I235" s="11" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="J235" t="s">
         <v>529</v>
@@ -12237,7 +12251,7 @@
         <v>1112</v>
       </c>
       <c r="I236" s="11" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="J236" t="s">
         <v>529</v>
@@ -12263,7 +12277,7 @@
         <v>1224</v>
       </c>
       <c r="I237" s="11" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
       <c r="J237" t="s">
         <v>528</v>
@@ -12289,7 +12303,7 @@
         <v>1225</v>
       </c>
       <c r="I238" s="11" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="J238" t="s">
         <v>528</v>
@@ -12341,7 +12355,7 @@
         <v>1227</v>
       </c>
       <c r="I240" s="11" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="J240" t="s">
         <v>528</v>
@@ -12367,7 +12381,7 @@
         <v>1228</v>
       </c>
       <c r="I241" s="11" t="s">
-        <v>1718</v>
+        <v>1716</v>
       </c>
       <c r="J241" t="s">
         <v>528</v>
@@ -12393,7 +12407,7 @@
         <v>1229</v>
       </c>
       <c r="I242" s="11" t="s">
-        <v>1719</v>
+        <v>1717</v>
       </c>
       <c r="J242" t="s">
         <v>528</v>
@@ -12419,7 +12433,7 @@
         <v>1230</v>
       </c>
       <c r="I243" s="11" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
       <c r="J243" t="s">
         <v>528</v>
@@ -12445,7 +12459,7 @@
         <v>1231</v>
       </c>
       <c r="I244" s="11" t="s">
-        <v>1721</v>
+        <v>1719</v>
       </c>
       <c r="J244" t="s">
         <v>528</v>
@@ -12497,7 +12511,7 @@
         <v>1233</v>
       </c>
       <c r="I246" s="11" t="s">
-        <v>1722</v>
+        <v>1720</v>
       </c>
       <c r="J246" t="s">
         <v>528</v>
@@ -12523,7 +12537,7 @@
         <v>1234</v>
       </c>
       <c r="I247" s="11" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="J247" t="s">
         <v>528</v>
@@ -12601,7 +12615,7 @@
         <v>1237</v>
       </c>
       <c r="I250" s="11" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
       <c r="J250" t="s">
         <v>528</v>
@@ -12627,7 +12641,7 @@
         <v>1238</v>
       </c>
       <c r="I251" s="11" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="J251" t="s">
         <v>528</v>
@@ -12653,7 +12667,7 @@
         <v>1239</v>
       </c>
       <c r="I252" s="11" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
       <c r="J252" t="s">
         <v>528</v>
@@ -12679,7 +12693,7 @@
         <v>1240</v>
       </c>
       <c r="I253" s="11" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
       <c r="J253" t="s">
         <v>528</v>
@@ -12705,7 +12719,7 @@
         <v>1241</v>
       </c>
       <c r="I254" s="11" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
       <c r="J254" t="s">
         <v>528</v>
@@ -12731,7 +12745,7 @@
         <v>1242</v>
       </c>
       <c r="I255" s="11" t="s">
-        <v>1729</v>
+        <v>1727</v>
       </c>
       <c r="J255" t="s">
         <v>528</v>
@@ -12757,7 +12771,7 @@
         <v>1243</v>
       </c>
       <c r="I256" s="11" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
       <c r="J256" t="s">
         <v>528</v>
@@ -12783,7 +12797,7 @@
         <v>1244</v>
       </c>
       <c r="I257" s="11" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
       <c r="J257" t="s">
         <v>528</v>
@@ -12809,7 +12823,7 @@
         <v>1245</v>
       </c>
       <c r="I258" s="11" t="s">
-        <v>1730</v>
+        <v>1728</v>
       </c>
       <c r="J258" t="s">
         <v>528</v>
@@ -12835,7 +12849,7 @@
         <v>1246</v>
       </c>
       <c r="I259" s="11" t="s">
-        <v>1731</v>
+        <v>1729</v>
       </c>
       <c r="J259" t="s">
         <v>528</v>
@@ -12861,7 +12875,7 @@
         <v>1247</v>
       </c>
       <c r="I260" s="11" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
       <c r="J260" t="s">
         <v>528</v>
@@ -12887,7 +12901,7 @@
         <v>1248</v>
       </c>
       <c r="I261" s="11" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
       <c r="J261" t="s">
         <v>528</v>
@@ -12913,7 +12927,7 @@
         <v>1249</v>
       </c>
       <c r="I262" s="11" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="J262" t="s">
         <v>528</v>
@@ -12939,7 +12953,7 @@
         <v>1250</v>
       </c>
       <c r="I263" s="11" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
       <c r="J263" t="s">
         <v>528</v>
@@ -12965,7 +12979,7 @@
         <v>1251</v>
       </c>
       <c r="I264" s="11" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
       <c r="J264" t="s">
         <v>528</v>
@@ -12991,7 +13005,7 @@
         <v>1252</v>
       </c>
       <c r="I265" s="11" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="J265" t="s">
         <v>528</v>
@@ -13017,7 +13031,7 @@
         <v>1253</v>
       </c>
       <c r="I266" s="11" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
       <c r="J266" t="s">
         <v>528</v>
@@ -13043,7 +13057,7 @@
         <v>1254</v>
       </c>
       <c r="I267" s="11" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="J267" t="s">
         <v>528</v>
@@ -13069,7 +13083,7 @@
         <v>1255</v>
       </c>
       <c r="I268" s="11" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="J268" t="s">
         <v>528</v>
@@ -13095,7 +13109,7 @@
         <v>1256</v>
       </c>
       <c r="I269" s="11" t="s">
-        <v>1740</v>
+        <v>1738</v>
       </c>
       <c r="J269" t="s">
         <v>528</v>
@@ -13121,7 +13135,7 @@
         <v>1257</v>
       </c>
       <c r="I270" s="11" t="s">
-        <v>1741</v>
+        <v>1739</v>
       </c>
       <c r="J270" t="s">
         <v>528</v>
@@ -13147,7 +13161,7 @@
         <v>1258</v>
       </c>
       <c r="I271" s="11" t="s">
-        <v>1742</v>
+        <v>1740</v>
       </c>
       <c r="J271" t="s">
         <v>528</v>
@@ -13173,7 +13187,7 @@
         <v>1259</v>
       </c>
       <c r="I272" s="11" t="s">
-        <v>1743</v>
+        <v>1741</v>
       </c>
       <c r="J272" t="s">
         <v>528</v>
@@ -13199,7 +13213,7 @@
         <v>1260</v>
       </c>
       <c r="I273" s="11" t="s">
-        <v>1744</v>
+        <v>1742</v>
       </c>
       <c r="J273" t="s">
         <v>528</v>
@@ -13225,7 +13239,7 @@
         <v>1261</v>
       </c>
       <c r="I274" s="11" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
       <c r="J274" t="s">
         <v>528</v>
@@ -13251,7 +13265,7 @@
         <v>1262</v>
       </c>
       <c r="I275" s="11" t="s">
-        <v>1884</v>
+        <v>1880</v>
       </c>
       <c r="J275" t="s">
         <v>528</v>
@@ -13277,7 +13291,7 @@
         <v>1263</v>
       </c>
       <c r="I276" s="11" t="s">
-        <v>1746</v>
+        <v>1744</v>
       </c>
       <c r="J276" t="s">
         <v>528</v>
@@ -13303,7 +13317,7 @@
         <v>1264</v>
       </c>
       <c r="I277" s="11" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="J277" t="s">
         <v>528</v>
@@ -13329,7 +13343,7 @@
         <v>1265</v>
       </c>
       <c r="I278" s="11" t="s">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="J278" t="s">
         <v>528</v>
@@ -13355,7 +13369,7 @@
         <v>1266</v>
       </c>
       <c r="I279" s="11" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
       <c r="J279" t="s">
         <v>528</v>
@@ -13381,7 +13395,7 @@
         <v>1267</v>
       </c>
       <c r="I280" s="11" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
       <c r="J280" t="s">
         <v>528</v>
@@ -13407,7 +13421,7 @@
         <v>1268</v>
       </c>
       <c r="I281" s="11" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
       <c r="J281" t="s">
         <v>528</v>
@@ -13433,7 +13447,7 @@
         <v>1269</v>
       </c>
       <c r="I282" s="11" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="J282" t="s">
         <v>528</v>
@@ -13459,7 +13473,7 @@
         <v>1270</v>
       </c>
       <c r="I283" s="11" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
       <c r="J283" t="s">
         <v>528</v>
@@ -13485,7 +13499,7 @@
         <v>1271</v>
       </c>
       <c r="I284" s="11" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
       <c r="J284" t="s">
         <v>528</v>
@@ -13511,7 +13525,7 @@
         <v>1272</v>
       </c>
       <c r="I285" s="11" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="J285" t="s">
         <v>528</v>
@@ -13537,7 +13551,7 @@
         <v>1273</v>
       </c>
       <c r="I286" s="11" t="s">
-        <v>1756</v>
+        <v>1886</v>
       </c>
       <c r="J286" t="s">
         <v>528</v>
@@ -13563,7 +13577,7 @@
         <v>1274</v>
       </c>
       <c r="I287" s="11" t="s">
-        <v>1757</v>
+        <v>1754</v>
       </c>
       <c r="J287" t="s">
         <v>528</v>
@@ -13589,7 +13603,7 @@
         <v>1275</v>
       </c>
       <c r="I288" s="11" t="s">
-        <v>1758</v>
+        <v>1755</v>
       </c>
       <c r="J288" t="s">
         <v>528</v>
@@ -13641,7 +13655,7 @@
         <v>1277</v>
       </c>
       <c r="I290" s="11" t="s">
-        <v>1759</v>
+        <v>1756</v>
       </c>
       <c r="J290" t="s">
         <v>530</v>
@@ -13667,7 +13681,7 @@
         <v>1278</v>
       </c>
       <c r="I291" s="11" t="s">
-        <v>1760</v>
+        <v>1757</v>
       </c>
       <c r="J291" t="s">
         <v>530</v>
@@ -13693,7 +13707,7 @@
         <v>1279</v>
       </c>
       <c r="I292" s="11" t="s">
-        <v>1761</v>
+        <v>1758</v>
       </c>
       <c r="J292" t="s">
         <v>530</v>
@@ -13719,7 +13733,7 @@
         <v>1092</v>
       </c>
       <c r="I293" s="11" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="J293" t="s">
         <v>530</v>
@@ -13745,7 +13759,7 @@
         <v>1280</v>
       </c>
       <c r="I294" s="11" t="s">
-        <v>1762</v>
+        <v>1759</v>
       </c>
       <c r="J294" t="s">
         <v>530</v>
@@ -13771,7 +13785,7 @@
         <v>1281</v>
       </c>
       <c r="I295" s="11" t="s">
-        <v>1763</v>
+        <v>1887</v>
       </c>
       <c r="J295" t="s">
         <v>530</v>
@@ -13797,7 +13811,7 @@
         <v>1282</v>
       </c>
       <c r="I296" s="11" t="s">
-        <v>1764</v>
+        <v>1760</v>
       </c>
       <c r="J296" t="s">
         <v>530</v>
@@ -13823,7 +13837,7 @@
         <v>1283</v>
       </c>
       <c r="I297" s="11" t="s">
-        <v>1765</v>
+        <v>1761</v>
       </c>
       <c r="J297" t="s">
         <v>530</v>
@@ -13849,7 +13863,7 @@
         <v>1284</v>
       </c>
       <c r="I298" s="11" t="s">
-        <v>1766</v>
+        <v>1762</v>
       </c>
       <c r="J298" t="s">
         <v>530</v>
@@ -13875,7 +13889,7 @@
         <v>1285</v>
       </c>
       <c r="I299" s="11" t="s">
-        <v>1767</v>
+        <v>1763</v>
       </c>
       <c r="J299" t="s">
         <v>530</v>
@@ -13901,7 +13915,7 @@
         <v>1286</v>
       </c>
       <c r="I300" s="11" t="s">
-        <v>1768</v>
+        <v>1764</v>
       </c>
       <c r="J300" t="s">
         <v>530</v>
@@ -13927,7 +13941,7 @@
         <v>1287</v>
       </c>
       <c r="I301" s="11" t="s">
-        <v>1769</v>
+        <v>1765</v>
       </c>
       <c r="J301" t="s">
         <v>530</v>
@@ -13953,7 +13967,7 @@
         <v>1288</v>
       </c>
       <c r="I302" s="11" t="s">
-        <v>1770</v>
+        <v>1766</v>
       </c>
       <c r="J302" t="s">
         <v>530</v>
@@ -13979,7 +13993,7 @@
         <v>1289</v>
       </c>
       <c r="I303" s="11" t="s">
-        <v>1771</v>
+        <v>1767</v>
       </c>
       <c r="J303" t="s">
         <v>530</v>
@@ -14005,7 +14019,7 @@
         <v>1290</v>
       </c>
       <c r="I304" s="11" t="s">
-        <v>1772</v>
+        <v>1768</v>
       </c>
       <c r="J304" t="s">
         <v>530</v>
@@ -14031,7 +14045,7 @@
         <v>1291</v>
       </c>
       <c r="I305" s="11" t="s">
-        <v>1773</v>
+        <v>1769</v>
       </c>
       <c r="J305" t="s">
         <v>530</v>
@@ -14057,7 +14071,7 @@
         <v>1292</v>
       </c>
       <c r="I306" s="11" t="s">
-        <v>1774</v>
+        <v>1770</v>
       </c>
       <c r="J306" t="s">
         <v>530</v>
@@ -14083,7 +14097,7 @@
         <v>1213</v>
       </c>
       <c r="I307" s="11" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="J307" t="s">
         <v>530</v>
@@ -14109,7 +14123,7 @@
         <v>1293</v>
       </c>
       <c r="I308" s="11" t="s">
-        <v>1775</v>
+        <v>1771</v>
       </c>
       <c r="J308" t="s">
         <v>530</v>
@@ -14135,7 +14149,7 @@
         <v>1294</v>
       </c>
       <c r="I309" s="11" t="s">
-        <v>1776</v>
+        <v>1772</v>
       </c>
       <c r="J309" t="s">
         <v>530</v>
@@ -14161,7 +14175,7 @@
         <v>1295</v>
       </c>
       <c r="I310" s="11" t="s">
-        <v>1777</v>
+        <v>1773</v>
       </c>
       <c r="J310" t="s">
         <v>530</v>
@@ -14187,7 +14201,7 @@
         <v>1296</v>
       </c>
       <c r="I311" s="11" t="s">
-        <v>1778</v>
+        <v>1774</v>
       </c>
       <c r="J311" t="s">
         <v>530</v>
@@ -14213,7 +14227,7 @@
         <v>1297</v>
       </c>
       <c r="I312" s="11" t="s">
-        <v>1779</v>
+        <v>1775</v>
       </c>
       <c r="J312" t="s">
         <v>530</v>
@@ -14239,7 +14253,7 @@
         <v>1298</v>
       </c>
       <c r="I313" s="11" t="s">
-        <v>1780</v>
+        <v>1776</v>
       </c>
       <c r="J313" t="s">
         <v>530</v>
@@ -14265,7 +14279,7 @@
         <v>1084</v>
       </c>
       <c r="I314" s="11" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="J314" t="s">
         <v>530</v>
@@ -14291,7 +14305,7 @@
         <v>1299</v>
       </c>
       <c r="I315" s="11" t="s">
-        <v>1781</v>
+        <v>1777</v>
       </c>
       <c r="J315" t="s">
         <v>530</v>
@@ -14317,7 +14331,7 @@
         <v>1300</v>
       </c>
       <c r="I316" s="11" t="s">
-        <v>1782</v>
+        <v>1778</v>
       </c>
       <c r="J316" t="s">
         <v>530</v>
@@ -14343,7 +14357,7 @@
         <v>1301</v>
       </c>
       <c r="I317" s="11" t="s">
-        <v>1783</v>
+        <v>1779</v>
       </c>
       <c r="J317" t="s">
         <v>530</v>
@@ -14369,7 +14383,7 @@
         <v>1302</v>
       </c>
       <c r="I318" s="11" t="s">
-        <v>1784</v>
+        <v>1780</v>
       </c>
       <c r="J318" t="s">
         <v>530</v>
@@ -14395,7 +14409,7 @@
         <v>1303</v>
       </c>
       <c r="I319" s="11" t="s">
-        <v>1785</v>
+        <v>1781</v>
       </c>
       <c r="J319" t="s">
         <v>530</v>
@@ -14421,7 +14435,7 @@
         <v>1304</v>
       </c>
       <c r="I320" s="11" t="s">
-        <v>1786</v>
+        <v>1782</v>
       </c>
       <c r="J320" t="s">
         <v>530</v>
@@ -14473,7 +14487,7 @@
         <v>1306</v>
       </c>
       <c r="I322" s="11" t="s">
-        <v>1787</v>
+        <v>1783</v>
       </c>
       <c r="J322" t="s">
         <v>530</v>
@@ -14499,7 +14513,7 @@
         <v>1307</v>
       </c>
       <c r="I323" s="11" t="s">
-        <v>1788</v>
+        <v>1784</v>
       </c>
       <c r="J323" t="s">
         <v>530</v>
@@ -14525,7 +14539,7 @@
         <v>1308</v>
       </c>
       <c r="I324" s="11" t="s">
-        <v>1789</v>
+        <v>1785</v>
       </c>
       <c r="J324" t="s">
         <v>530</v>
@@ -14551,7 +14565,7 @@
         <v>1309</v>
       </c>
       <c r="I325" s="11" t="s">
-        <v>1790</v>
+        <v>1786</v>
       </c>
       <c r="J325" t="s">
         <v>530</v>
@@ -14577,7 +14591,7 @@
         <v>1310</v>
       </c>
       <c r="I326" s="11" t="s">
-        <v>1791</v>
+        <v>1787</v>
       </c>
       <c r="J326" t="s">
         <v>530</v>
@@ -14603,7 +14617,7 @@
         <v>1311</v>
       </c>
       <c r="I327" s="11" t="s">
-        <v>1792</v>
+        <v>1788</v>
       </c>
       <c r="J327" t="s">
         <v>530</v>
@@ -14655,7 +14669,7 @@
         <v>1313</v>
       </c>
       <c r="I329" s="11" t="s">
-        <v>1793</v>
+        <v>1789</v>
       </c>
       <c r="J329" t="s">
         <v>530</v>
@@ -14681,7 +14695,7 @@
         <v>1314</v>
       </c>
       <c r="I330" s="11" t="s">
-        <v>1794</v>
+        <v>1790</v>
       </c>
       <c r="J330" t="s">
         <v>530</v>
@@ -14707,7 +14721,7 @@
         <v>1315</v>
       </c>
       <c r="I331" s="11" t="s">
-        <v>1795</v>
+        <v>1791</v>
       </c>
       <c r="J331" t="s">
         <v>530</v>
@@ -14733,7 +14747,7 @@
         <v>1316</v>
       </c>
       <c r="I332" s="11" t="s">
-        <v>1796</v>
+        <v>1792</v>
       </c>
       <c r="J332" t="s">
         <v>530</v>
@@ -14759,7 +14773,7 @@
         <v>1317</v>
       </c>
       <c r="I333" s="11" t="s">
-        <v>1797</v>
+        <v>1793</v>
       </c>
       <c r="J333" t="s">
         <v>530</v>
@@ -14785,7 +14799,7 @@
         <v>1318</v>
       </c>
       <c r="I334" s="11" t="s">
-        <v>1798</v>
+        <v>1794</v>
       </c>
       <c r="J334" t="s">
         <v>530</v>
@@ -14811,7 +14825,7 @@
         <v>1319</v>
       </c>
       <c r="I335" s="11" t="s">
-        <v>1799</v>
+        <v>1795</v>
       </c>
       <c r="J335" t="s">
         <v>530</v>
@@ -14837,7 +14851,7 @@
         <v>1320</v>
       </c>
       <c r="I336" s="11" t="s">
-        <v>1800</v>
+        <v>1796</v>
       </c>
       <c r="J336" t="s">
         <v>530</v>
@@ -14863,7 +14877,7 @@
         <v>1321</v>
       </c>
       <c r="I337" s="11" t="s">
-        <v>1801</v>
+        <v>1797</v>
       </c>
       <c r="J337" t="s">
         <v>530</v>
@@ -14889,7 +14903,7 @@
         <v>1322</v>
       </c>
       <c r="I338" s="11" t="s">
-        <v>1802</v>
+        <v>1798</v>
       </c>
       <c r="J338" t="s">
         <v>530</v>
@@ -14915,7 +14929,7 @@
         <v>1323</v>
       </c>
       <c r="I339" s="11" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="J339" t="s">
         <v>530</v>
@@ -14941,7 +14955,7 @@
         <v>1324</v>
       </c>
       <c r="I340" s="11" t="s">
-        <v>1803</v>
+        <v>1799</v>
       </c>
       <c r="J340" t="s">
         <v>530</v>
@@ -14967,7 +14981,7 @@
         <v>1325</v>
       </c>
       <c r="I341" s="11" t="s">
-        <v>1804</v>
+        <v>1800</v>
       </c>
       <c r="J341" t="s">
         <v>530</v>
@@ -14993,7 +15007,7 @@
         <v>1326</v>
       </c>
       <c r="I342" s="11" t="s">
-        <v>1805</v>
+        <v>1801</v>
       </c>
       <c r="J342" t="s">
         <v>530</v>
@@ -15019,7 +15033,7 @@
         <v>1327</v>
       </c>
       <c r="I343" s="11" t="s">
-        <v>1806</v>
+        <v>1802</v>
       </c>
       <c r="J343" t="s">
         <v>530</v>
@@ -15045,7 +15059,7 @@
         <v>1328</v>
       </c>
       <c r="I344" s="11" t="s">
-        <v>1807</v>
+        <v>1803</v>
       </c>
       <c r="J344" t="s">
         <v>530</v>
@@ -15071,7 +15085,7 @@
         <v>1329</v>
       </c>
       <c r="I345" s="11" t="s">
-        <v>1808</v>
+        <v>1804</v>
       </c>
       <c r="J345" t="s">
         <v>530</v>
@@ -15097,7 +15111,7 @@
         <v>1330</v>
       </c>
       <c r="I346" s="11" t="s">
-        <v>1809</v>
+        <v>1805</v>
       </c>
       <c r="J346" t="s">
         <v>530</v>
@@ -15123,7 +15137,7 @@
         <v>1331</v>
       </c>
       <c r="I347" s="11" t="s">
-        <v>1810</v>
+        <v>1806</v>
       </c>
       <c r="J347" t="s">
         <v>530</v>
@@ -15149,7 +15163,7 @@
         <v>1332</v>
       </c>
       <c r="I348" s="11" t="s">
-        <v>1811</v>
+        <v>1807</v>
       </c>
       <c r="J348" t="s">
         <v>530</v>
@@ -15175,7 +15189,7 @@
         <v>1333</v>
       </c>
       <c r="I349" s="11" t="s">
-        <v>1812</v>
+        <v>1808</v>
       </c>
       <c r="J349" t="s">
         <v>530</v>
@@ -15201,7 +15215,7 @@
         <v>1334</v>
       </c>
       <c r="I350" s="11" t="s">
-        <v>1813</v>
+        <v>1809</v>
       </c>
       <c r="J350" t="s">
         <v>530</v>
@@ -15227,7 +15241,7 @@
         <v>1335</v>
       </c>
       <c r="I351" s="11" t="s">
-        <v>1814</v>
+        <v>1810</v>
       </c>
       <c r="J351" t="s">
         <v>530</v>
@@ -15253,7 +15267,7 @@
         <v>1336</v>
       </c>
       <c r="I352" s="11" t="s">
-        <v>1815</v>
+        <v>1811</v>
       </c>
       <c r="J352" t="s">
         <v>530</v>
@@ -15305,7 +15319,7 @@
         <v>1338</v>
       </c>
       <c r="I354" s="11" t="s">
-        <v>1816</v>
+        <v>1812</v>
       </c>
       <c r="J354" t="s">
         <v>530</v>
@@ -15331,7 +15345,7 @@
         <v>1339</v>
       </c>
       <c r="I355" s="11" t="s">
-        <v>1817</v>
+        <v>1813</v>
       </c>
       <c r="J355" t="s">
         <v>530</v>
@@ -15357,7 +15371,7 @@
         <v>1340</v>
       </c>
       <c r="I356" s="11" t="s">
-        <v>1818</v>
+        <v>1814</v>
       </c>
       <c r="J356" t="s">
         <v>530</v>
@@ -15383,7 +15397,7 @@
         <v>1341</v>
       </c>
       <c r="I357" s="11" t="s">
-        <v>1819</v>
+        <v>1815</v>
       </c>
       <c r="J357" t="s">
         <v>530</v>
@@ -15409,7 +15423,7 @@
         <v>1342</v>
       </c>
       <c r="I358" s="11" t="s">
-        <v>1820</v>
+        <v>1816</v>
       </c>
       <c r="J358" t="s">
         <v>530</v>
@@ -15435,7 +15449,7 @@
         <v>1343</v>
       </c>
       <c r="I359" s="11" t="s">
-        <v>1821</v>
+        <v>1817</v>
       </c>
       <c r="J359" t="s">
         <v>530</v>
@@ -15461,7 +15475,7 @@
         <v>1344</v>
       </c>
       <c r="I360" s="11" t="s">
-        <v>1822</v>
+        <v>1818</v>
       </c>
       <c r="J360" t="s">
         <v>530</v>
@@ -15487,7 +15501,7 @@
         <v>1345</v>
       </c>
       <c r="I361" s="11" t="s">
-        <v>1823</v>
+        <v>1819</v>
       </c>
       <c r="J361" t="s">
         <v>530</v>
@@ -15513,7 +15527,7 @@
         <v>1346</v>
       </c>
       <c r="I362" s="11" t="s">
-        <v>1824</v>
+        <v>1820</v>
       </c>
       <c r="J362" t="s">
         <v>530</v>
@@ -15539,7 +15553,7 @@
         <v>1347</v>
       </c>
       <c r="I363" s="11" t="s">
-        <v>1825</v>
+        <v>1821</v>
       </c>
       <c r="J363" t="s">
         <v>530</v>
@@ -15565,7 +15579,7 @@
         <v>1348</v>
       </c>
       <c r="I364" s="11" t="s">
-        <v>1826</v>
+        <v>1822</v>
       </c>
       <c r="J364" t="s">
         <v>530</v>
@@ -15591,7 +15605,7 @@
         <v>1349</v>
       </c>
       <c r="I365" s="11" t="s">
-        <v>1827</v>
+        <v>1823</v>
       </c>
       <c r="J365" t="s">
         <v>530</v>
@@ -15617,7 +15631,7 @@
         <v>1350</v>
       </c>
       <c r="I366" s="11" t="s">
-        <v>1828</v>
+        <v>1824</v>
       </c>
       <c r="J366" t="s">
         <v>530</v>
@@ -15643,7 +15657,7 @@
         <v>1351</v>
       </c>
       <c r="I367" s="11" t="s">
-        <v>1829</v>
+        <v>1825</v>
       </c>
       <c r="J367" t="s">
         <v>530</v>
@@ -15669,7 +15683,7 @@
         <v>1352</v>
       </c>
       <c r="I368" s="11" t="s">
-        <v>1830</v>
+        <v>1826</v>
       </c>
       <c r="J368" t="s">
         <v>530</v>
@@ -15695,7 +15709,7 @@
         <v>1353</v>
       </c>
       <c r="I369" s="11" t="s">
-        <v>1831</v>
+        <v>1827</v>
       </c>
       <c r="J369" t="s">
         <v>530</v>
@@ -15721,7 +15735,7 @@
         <v>1354</v>
       </c>
       <c r="I370" s="11" t="s">
-        <v>1832</v>
+        <v>1828</v>
       </c>
       <c r="J370" t="s">
         <v>530</v>
@@ -15747,7 +15761,7 @@
         <v>1355</v>
       </c>
       <c r="I371" s="11" t="s">
-        <v>1833</v>
+        <v>1829</v>
       </c>
       <c r="J371" t="s">
         <v>530</v>
@@ -15773,7 +15787,7 @@
         <v>1356</v>
       </c>
       <c r="I372" s="11" t="s">
-        <v>1834</v>
+        <v>1830</v>
       </c>
       <c r="J372" t="s">
         <v>530</v>
@@ -15799,7 +15813,7 @@
         <v>1357</v>
       </c>
       <c r="I373" s="11" t="s">
-        <v>1835</v>
+        <v>1831</v>
       </c>
       <c r="J373" t="s">
         <v>530</v>
@@ -15825,7 +15839,7 @@
         <v>1358</v>
       </c>
       <c r="I374" s="11" t="s">
-        <v>1836</v>
+        <v>1832</v>
       </c>
       <c r="J374" t="s">
         <v>530</v>
@@ -15851,7 +15865,7 @@
         <v>1359</v>
       </c>
       <c r="I375" s="11" t="s">
-        <v>1837</v>
+        <v>1833</v>
       </c>
       <c r="J375" t="s">
         <v>530</v>
@@ -15877,7 +15891,7 @@
         <v>1360</v>
       </c>
       <c r="I376" s="11" t="s">
-        <v>1838</v>
+        <v>1834</v>
       </c>
       <c r="J376" t="s">
         <v>530</v>
@@ -15903,7 +15917,7 @@
         <v>1361</v>
       </c>
       <c r="I377" s="11" t="s">
-        <v>1839</v>
+        <v>1835</v>
       </c>
       <c r="J377" t="s">
         <v>530</v>
@@ -15929,7 +15943,7 @@
         <v>1362</v>
       </c>
       <c r="I378" s="11" t="s">
-        <v>1840</v>
+        <v>1836</v>
       </c>
       <c r="J378" t="s">
         <v>528</v>
@@ -15955,7 +15969,7 @@
         <v>1363</v>
       </c>
       <c r="I379" s="11" t="s">
-        <v>1841</v>
+        <v>1837</v>
       </c>
       <c r="J379" t="s">
         <v>528</v>
@@ -15981,7 +15995,7 @@
         <v>1364</v>
       </c>
       <c r="I380" s="11" t="s">
-        <v>1842</v>
+        <v>1838</v>
       </c>
       <c r="J380" t="s">
         <v>528</v>
@@ -16007,7 +16021,7 @@
         <v>1365</v>
       </c>
       <c r="I381" s="11" t="s">
-        <v>1843</v>
+        <v>1839</v>
       </c>
       <c r="J381" t="s">
         <v>528</v>
@@ -16033,7 +16047,7 @@
         <v>1366</v>
       </c>
       <c r="I382" s="11" t="s">
-        <v>1844</v>
+        <v>1840</v>
       </c>
       <c r="J382" t="s">
         <v>528</v>
@@ -16059,7 +16073,7 @@
         <v>1367</v>
       </c>
       <c r="I383" s="11" t="s">
-        <v>1845</v>
+        <v>1841</v>
       </c>
       <c r="J383" t="s">
         <v>528</v>
@@ -16085,7 +16099,7 @@
         <v>1368</v>
       </c>
       <c r="I384" s="11" t="s">
-        <v>1846</v>
+        <v>1842</v>
       </c>
       <c r="J384" t="s">
         <v>528</v>
@@ -16111,7 +16125,7 @@
         <v>1369</v>
       </c>
       <c r="I385" s="11" t="s">
-        <v>1847</v>
+        <v>1843</v>
       </c>
       <c r="J385" t="s">
         <v>528</v>
@@ -16137,7 +16151,7 @@
         <v>1370</v>
       </c>
       <c r="I386" s="11" t="s">
-        <v>1848</v>
+        <v>1844</v>
       </c>
       <c r="J386" t="s">
         <v>531</v>
@@ -16163,7 +16177,7 @@
         <v>1371</v>
       </c>
       <c r="I387" s="11" t="s">
-        <v>1849</v>
+        <v>1845</v>
       </c>
       <c r="J387" t="s">
         <v>531</v>
@@ -16189,7 +16203,7 @@
         <v>1372</v>
       </c>
       <c r="I388" s="11" t="s">
-        <v>1850</v>
+        <v>1846</v>
       </c>
       <c r="J388" t="s">
         <v>531</v>
@@ -16215,7 +16229,7 @@
         <v>1373</v>
       </c>
       <c r="I389" s="11" t="s">
-        <v>1849</v>
+        <v>1845</v>
       </c>
       <c r="J389" t="s">
         <v>531</v>
@@ -16241,7 +16255,7 @@
         <v>1374</v>
       </c>
       <c r="I390" s="11" t="s">
-        <v>1851</v>
+        <v>1847</v>
       </c>
       <c r="J390" t="s">
         <v>531</v>
@@ -16267,7 +16281,7 @@
         <v>1375</v>
       </c>
       <c r="I391" s="11" t="s">
-        <v>1852</v>
+        <v>1848</v>
       </c>
       <c r="J391" t="s">
         <v>531</v>
@@ -16293,7 +16307,7 @@
         <v>1376</v>
       </c>
       <c r="I392" s="11" t="s">
-        <v>1853</v>
+        <v>1849</v>
       </c>
       <c r="J392" t="s">
         <v>531</v>
@@ -16319,7 +16333,7 @@
         <v>1377</v>
       </c>
       <c r="I393" s="11" t="s">
-        <v>1854</v>
+        <v>1850</v>
       </c>
       <c r="J393" t="s">
         <v>531</v>
@@ -16345,7 +16359,7 @@
         <v>1378</v>
       </c>
       <c r="I394" s="11" t="s">
-        <v>1855</v>
+        <v>1851</v>
       </c>
       <c r="J394" t="s">
         <v>531</v>
@@ -16371,7 +16385,7 @@
         <v>1379</v>
       </c>
       <c r="I395" s="11" t="s">
-        <v>1856</v>
+        <v>1852</v>
       </c>
       <c r="J395" t="s">
         <v>531</v>
@@ -16397,7 +16411,7 @@
         <v>1380</v>
       </c>
       <c r="I396" s="11" t="s">
-        <v>1857</v>
+        <v>1853</v>
       </c>
       <c r="J396" t="s">
         <v>531</v>
@@ -16423,7 +16437,7 @@
         <v>1381</v>
       </c>
       <c r="I397" s="11" t="s">
-        <v>1858</v>
+        <v>1854</v>
       </c>
       <c r="J397" t="s">
         <v>531</v>
@@ -16449,7 +16463,7 @@
         <v>1382</v>
       </c>
       <c r="I398" s="11" t="s">
-        <v>1859</v>
+        <v>1855</v>
       </c>
       <c r="J398" t="s">
         <v>531</v>
@@ -16475,7 +16489,7 @@
         <v>1383</v>
       </c>
       <c r="I399" s="11" t="s">
-        <v>1860</v>
+        <v>1856</v>
       </c>
       <c r="J399" t="s">
         <v>531</v>
@@ -16501,7 +16515,7 @@
         <v>1384</v>
       </c>
       <c r="I400" s="11" t="s">
-        <v>1861</v>
+        <v>1857</v>
       </c>
       <c r="J400" t="s">
         <v>531</v>
@@ -16527,7 +16541,7 @@
         <v>1385</v>
       </c>
       <c r="I401" s="11" t="s">
-        <v>1862</v>
+        <v>1858</v>
       </c>
       <c r="J401" t="s">
         <v>531</v>
@@ -16553,7 +16567,7 @@
         <v>1386</v>
       </c>
       <c r="I402" s="11" t="s">
-        <v>1863</v>
+        <v>1859</v>
       </c>
       <c r="J402" t="s">
         <v>531</v>
@@ -16579,7 +16593,7 @@
         <v>1387</v>
       </c>
       <c r="I403" s="11" t="s">
-        <v>1864</v>
+        <v>1860</v>
       </c>
       <c r="J403" t="s">
         <v>531</v>
@@ -16605,7 +16619,7 @@
         <v>1388</v>
       </c>
       <c r="I404" s="11" t="s">
-        <v>1865</v>
+        <v>1861</v>
       </c>
       <c r="J404" t="s">
         <v>531</v>
@@ -16631,7 +16645,7 @@
         <v>1389</v>
       </c>
       <c r="I405" s="11" t="s">
-        <v>1806</v>
+        <v>1802</v>
       </c>
       <c r="J405" t="s">
         <v>531</v>
@@ -16657,7 +16671,7 @@
         <v>1390</v>
       </c>
       <c r="I406" s="11" t="s">
-        <v>1866</v>
+        <v>1862</v>
       </c>
       <c r="J406" t="s">
         <v>531</v>
@@ -16683,7 +16697,7 @@
         <v>1391</v>
       </c>
       <c r="I407" s="11" t="s">
-        <v>1867</v>
+        <v>1863</v>
       </c>
       <c r="J407" t="s">
         <v>531</v>
@@ -16709,7 +16723,7 @@
         <v>1392</v>
       </c>
       <c r="I408" s="11" t="s">
-        <v>1867</v>
+        <v>1863</v>
       </c>
       <c r="J408" t="s">
         <v>531</v>
@@ -16735,7 +16749,7 @@
         <v>1393</v>
       </c>
       <c r="I409" s="11" t="s">
-        <v>1867</v>
+        <v>1863</v>
       </c>
       <c r="J409" t="s">
         <v>531</v>
@@ -16761,7 +16775,7 @@
         <v>1394</v>
       </c>
       <c r="I410" s="11" t="s">
-        <v>1868</v>
+        <v>1864</v>
       </c>
       <c r="J410" t="s">
         <v>531</v>
@@ -16787,7 +16801,7 @@
         <v>1395</v>
       </c>
       <c r="I411" s="11" t="s">
-        <v>1869</v>
+        <v>1865</v>
       </c>
       <c r="J411" t="s">
         <v>531</v>
@@ -16813,7 +16827,7 @@
         <v>1396</v>
       </c>
       <c r="I412" s="11" t="s">
-        <v>1869</v>
+        <v>1865</v>
       </c>
       <c r="J412" t="s">
         <v>531</v>
@@ -16839,7 +16853,7 @@
         <v>1397</v>
       </c>
       <c r="I413" s="11" t="s">
-        <v>1870</v>
+        <v>1866</v>
       </c>
       <c r="J413" t="s">
         <v>531</v>
@@ -16865,7 +16879,7 @@
         <v>1398</v>
       </c>
       <c r="I414" s="11" t="s">
-        <v>1870</v>
+        <v>1866</v>
       </c>
       <c r="J414" t="s">
         <v>531</v>
@@ -16891,7 +16905,7 @@
         <v>1399</v>
       </c>
       <c r="I415" s="11" t="s">
-        <v>1871</v>
+        <v>1867</v>
       </c>
       <c r="J415" t="s">
         <v>531</v>
@@ -16943,7 +16957,7 @@
         <v>1401</v>
       </c>
       <c r="I417" s="11" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="J417" t="s">
         <v>531</v>
@@ -16969,7 +16983,7 @@
         <v>1223</v>
       </c>
       <c r="I418" s="11" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="J418" t="s">
         <v>531</v>
@@ -16995,7 +17009,7 @@
         <v>1402</v>
       </c>
       <c r="I419" s="11" t="s">
-        <v>1872</v>
+        <v>1868</v>
       </c>
       <c r="J419" t="s">
         <v>531</v>
@@ -17021,7 +17035,7 @@
         <v>1403</v>
       </c>
       <c r="I420" s="11" t="s">
-        <v>1873</v>
+        <v>1869</v>
       </c>
       <c r="J420" t="s">
         <v>531</v>
@@ -17047,7 +17061,7 @@
         <v>1264</v>
       </c>
       <c r="I421" s="11" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="J421" t="s">
         <v>531</v>
@@ -17073,7 +17087,7 @@
         <v>1404</v>
       </c>
       <c r="I422" s="11" t="s">
-        <v>1874</v>
+        <v>1870</v>
       </c>
       <c r="J422" t="s">
         <v>531</v>
@@ -17099,7 +17113,7 @@
         <v>1405</v>
       </c>
       <c r="I423" s="11" t="s">
-        <v>1875</v>
+        <v>1871</v>
       </c>
       <c r="J423" t="s">
         <v>531</v>
@@ -17125,7 +17139,7 @@
         <v>1406</v>
       </c>
       <c r="I424" s="11" t="s">
-        <v>1876</v>
+        <v>1872</v>
       </c>
       <c r="J424" t="s">
         <v>531</v>
@@ -17151,7 +17165,7 @@
         <v>1407</v>
       </c>
       <c r="I425" s="11" t="s">
-        <v>1877</v>
+        <v>1873</v>
       </c>
       <c r="J425" t="s">
         <v>531</v>
@@ -17177,7 +17191,7 @@
         <v>1408</v>
       </c>
       <c r="I426" s="11" t="s">
-        <v>1878</v>
+        <v>1874</v>
       </c>
       <c r="J426" t="s">
         <v>531</v>
@@ -17203,7 +17217,7 @@
         <v>1409</v>
       </c>
       <c r="I427" s="11" t="s">
-        <v>1879</v>
+        <v>1875</v>
       </c>
       <c r="J427" t="s">
         <v>531</v>

</xml_diff>

<commit_message>
Norwegian WG uni_lemma change
</commit_message>
<xml_diff>
--- a/raw_data/Norwegian_WG/[Norwegian_WG].xlsx
+++ b/raw_data/Norwegian_WG/[Norwegian_WG].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="13040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -5947,8 +5947,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -6132,7 +6152,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="179">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -6212,6 +6232,16 @@
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6291,6 +6321,16 @@
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6622,8 +6662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J490"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
+      <selection activeCell="F419" sqref="F419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -17390,7 +17430,7 @@
         <v>1500</v>
       </c>
       <c r="F418" s="10" t="s">
-        <v>515</v>
+        <v>1678</v>
       </c>
       <c r="G418" s="10" t="s">
         <v>1217</v>

</xml_diff>